<commit_message>
Modified CD3 templates for exa-vmclusters
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop_new\oci_tools\cd3_automation_toolkit\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop\oci_tools\cd3_automation_toolkit\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="545">
   <si>
     <t>Region</t>
   </si>
@@ -5597,6 +5597,9 @@
       <t xml:space="preserve"> PHXNonProd-VCN_ngw)
 </t>
     </r>
+  </si>
+  <si>
+    <t>Backup Network NSGs</t>
   </si>
 </sst>
 </file>
@@ -6143,7 +6146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6469,6 +6472,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -32567,7 +32577,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -32601,25 +32611,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="52" customFormat="1" ht="195" customHeight="1">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="122" t="s">
         <v>418</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="123"/>
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
       <c r="R1" s="95"/>
       <c r="S1" s="95"/>
       <c r="T1" s="95"/>
@@ -32671,11 +32681,15 @@
       <c r="N2" s="89" t="s">
         <v>416</v>
       </c>
-      <c r="O2" s="96" t="s">
+      <c r="O2" s="135" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" s="135" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q2" s="96" t="s">
         <v>273</v>
       </c>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
       <c r="R2" s="48"/>
       <c r="S2" s="48"/>
       <c r="T2" s="48"/>
@@ -32697,8 +32711,10 @@
       <c r="K3" s="53"/>
       <c r="L3" s="70"/>
       <c r="M3" s="53"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="36"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
     </row>
     <row r="4" spans="1:24" ht="14.5" customHeight="1">
       <c r="A4" s="100"/>
@@ -32714,8 +32730,9 @@
       <c r="K4" s="98"/>
       <c r="L4" s="99"/>
       <c r="M4" s="98"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="73"/>
+      <c r="N4" s="61"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="36"/>
     </row>
     <row r="5" spans="1:24" s="38" customFormat="1" ht="14.5" customHeight="1">
       <c r="A5" s="100"/>
@@ -32730,7 +32747,8 @@
       <c r="L5" s="61"/>
       <c r="M5" s="53"/>
       <c r="N5" s="61"/>
-      <c r="O5" s="36"/>
+      <c r="O5" s="136"/>
+      <c r="R5" s="103"/>
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="48"/>
@@ -39475,7 +39493,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G1048576">
@@ -39502,11 +39520,23 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select an OCI region">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;">
           <x14:formula1>
-            <xm:f>drop_down_rule_set!$G$2:$G$25</xm:f>
+            <xm:f>INDIRECT("drop_down_rule_set!$D$2:"&amp;ADDRESS(COUNTIF('D:\PycharmProjects\oci_develop_new\indir\[CD3-gc35008.xlsx]drop_down_rule_set'!#REF!,"*?")+1,4,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A1000</xm:sqref>
+          <xm:sqref>C6:C501</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_set!$D$2:"&amp;ADDRESS(COUNTIF('[CD3-DRGv2-template.xlsx]drop_down_rule_set'!#REF!,"*?")+1,4,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:F1000</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF('[CD3-DRGv2-template.xlsx]drop_down_rule_comp'!#REF!,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3:B1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
@@ -39514,23 +39544,11 @@
           </x14:formula1>
           <xm:sqref>D6:D501</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select an OCI region">
           <x14:formula1>
-            <xm:f>INDIRECT("drop_down_rule_set!$D$2:"&amp;ADDRESS(COUNTIF('D:\PycharmProjects\oci_develop_new\indir\[CD3-gc35008.xlsx]drop_down_rule_set'!#REF!,"*?")+1,4,1,4))</xm:f>
+            <xm:f>'[CD3-DRGv2-template.xlsx]drop_down_rule_set'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C6:C501</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
-          <x14:formula1>
-            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B500,"*?")+1,2,1,4))</xm:f>
-          </x14:formula1>
-          <xm:sqref>B3:B1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;">
-          <x14:formula1>
-            <xm:f>INDIRECT("drop_down_rule_set!$D$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_set!C$2:$D501,"*?")+1,4,1,4))</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3:F1000</xm:sqref>
+          <xm:sqref>A3:A1000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
DB Systems changes as per BMC export
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -117,7 +117,7 @@
     <definedName name="VM_Shapes" localSheetId="27">Database_Dropdown!$A$2:$A$12</definedName>
     <definedName name="VM_Shapes" localSheetId="10">#REF!</definedName>
     <definedName name="VM_Shapes" localSheetId="6">#REF!</definedName>
-    <definedName name="VM_Shapes">'DBSystems-VM-BM'!$AA$397:$AA$407</definedName>
+    <definedName name="VM_Shapes">'DBSystems-VM-BM'!$AB$397:$AB$407</definedName>
     <definedName name="VM_shapes_drop" localSheetId="10">[1]Database_Dropdown!$A$2:$A$7</definedName>
     <definedName name="VM_shapes_drop" localSheetId="6">[2]Database_Dropdown!$A$2:$A$7</definedName>
     <definedName name="VM_shapes_drop" localSheetId="30">[3]Database_Dropdown!$A$2:$A$7</definedName>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="545">
   <si>
     <t>Region</t>
   </si>
@@ -20139,10 +20139,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14.5"/>
@@ -20164,13 +20164,14 @@
     <col min="20" max="20" width="23" style="37" bestFit="1" customWidth="1"/>
     <col min="21" max="23" width="20.453125" style="37"/>
     <col min="24" max="24" width="23.1796875" style="37" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.1796875" style="37" customWidth="1"/>
-    <col min="26" max="26" width="20.453125" style="37"/>
-    <col min="27" max="27" width="23.1796875" style="37" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="20.453125" style="37"/>
+    <col min="25" max="25" width="17" style="37" customWidth="1"/>
+    <col min="26" max="26" width="10.54296875" style="37" customWidth="1"/>
+    <col min="27" max="27" width="20.453125" style="37"/>
+    <col min="28" max="28" width="23.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="20.453125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="52" customFormat="1" ht="135.75" customHeight="1">
+    <row r="1" spans="1:27" s="52" customFormat="1" ht="135.75" customHeight="1">
       <c r="A1" s="117" t="s">
         <v>417</v>
       </c>
@@ -20198,9 +20199,10 @@
       <c r="W1" s="118"/>
       <c r="X1" s="118"/>
       <c r="Y1" s="118"/>
-      <c r="Z1" s="119"/>
-    </row>
-    <row r="2" spans="1:26" s="63" customFormat="1" ht="43.5">
+      <c r="Z1" s="118"/>
+      <c r="AA1" s="119"/>
+    </row>
+    <row r="2" spans="1:27" s="63" customFormat="1" ht="43.5">
       <c r="A2" s="66" t="s">
         <v>0</v>
       </c>
@@ -20277,10 +20279,13 @@
         <v>416</v>
       </c>
       <c r="Z2" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA2" s="66" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:27">
       <c r="A3" s="38"/>
       <c r="B3" s="38"/>
       <c r="C3" s="30"/>
@@ -20307,8 +20312,9 @@
       <c r="X3" s="38"/>
       <c r="Y3" s="38"/>
       <c r="Z3" s="38"/>
-    </row>
-    <row r="4" spans="1:26">
+      <c r="AA3" s="38"/>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" s="100"/>
       <c r="B4" s="100"/>
       <c r="C4" s="100"/>
@@ -20335,8 +20341,9 @@
       <c r="X4" s="38"/>
       <c r="Y4" s="38"/>
       <c r="Z4" s="38"/>
-    </row>
-    <row r="5" spans="1:26">
+      <c r="AA4" s="38"/>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="102"/>
       <c r="B5" s="100"/>
       <c r="C5" s="100"/>
@@ -20363,8 +20370,9 @@
       <c r="X5" s="38"/>
       <c r="Y5" s="38"/>
       <c r="Z5" s="38"/>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="AA5" s="38"/>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" s="100"/>
       <c r="B6" s="100"/>
       <c r="C6" s="100"/>
@@ -20391,8 +20399,9 @@
       <c r="X6" s="38"/>
       <c r="Y6" s="38"/>
       <c r="Z6" s="38"/>
-    </row>
-    <row r="7" spans="1:26">
+      <c r="AA6" s="38"/>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" s="100"/>
       <c r="B7" s="100"/>
       <c r="C7" s="100"/>
@@ -20419,56 +20428,57 @@
       <c r="X7" s="38"/>
       <c r="Y7" s="38"/>
       <c r="Z7" s="38"/>
-    </row>
-    <row r="8" spans="1:26">
+      <c r="AA7" s="38"/>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8" s="48"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
       <c r="D8" s="57"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:27">
       <c r="A9" s="48"/>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
       <c r="D9" s="57"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:27">
       <c r="A10" s="48"/>
       <c r="B10" s="48"/>
       <c r="C10" s="48"/>
       <c r="D10" s="57"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:27">
       <c r="A11" s="48"/>
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
       <c r="D11" s="57"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:27">
       <c r="A12" s="48"/>
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="D12" s="57"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:27">
       <c r="A13" s="48"/>
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="57"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:27">
       <c r="A14" s="48"/>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="57"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:27">
       <c r="A15" s="48"/>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
       <c r="D15" s="57"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:27">
       <c r="A16" s="48"/>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
@@ -26380,47 +26390,29 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A1:AA1"/>
   </mergeCells>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S1001:S1048576">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S1048576">
       <formula1>workload_drop</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1001:F1048576">
       <formula1>VM_shapes_drop</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1001:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576">
       <formula1>software_drop</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1001:P1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P1048576">
       <formula1>db_sersion_drop</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1001:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M1048576">
       <formula1>license_type_drop</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1001:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3:V1048576">
       <formula1>char_set</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1001:W1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W1048576">
       <formula1>nchar_set</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W1000">
-      <formula1>nchar_set</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3:V1000">
-      <formula1>char_set</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S1000">
-      <formula1>workload_drop</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P1000">
-      <formula1>db_sersion_drop</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M1000">
-      <formula1>license_type_drop</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1000">
-      <formula1>software_drop</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32571,8 +32563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="G1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -46524,7 +46516,13 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="27">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify your tenancy's Home Region for creating IAM Policies.">
+          <x14:formula1>
+            <xm:f>drop_down_rule_set!$G$2:$G$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3:A530</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C656,"*?")+1,2,1,4))</xm:f>
@@ -46551,15 +46549,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C664,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C184</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C591,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C184 C111:C142</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify your tenancy's Home Region for creating IAM Policies.">
-          <x14:formula1>
-            <xm:f>drop_down_rule_set!$G$2:$G$25</xm:f>
-          </x14:formula1>
-          <xm:sqref>A3:A530</xm:sqref>
+          <xm:sqref>C111:C142</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
@@ -46569,33 +46567,87 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C598,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C106:C107</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C533,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C106:C107 C41:C43 C145:C146</xm:sqref>
+          <xm:sqref>C41:C43</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C637,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C145:C146</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C599,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C109 C148</xm:sqref>
+          <xm:sqref>C109</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C638,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C148</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C601,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C110</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C599,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C110 C108 C149 C147</xm:sqref>
+          <xm:sqref>C108</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C640,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C149</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C638,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C147</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C599,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C104 C143</xm:sqref>
+          <xm:sqref>C104</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C638,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C143</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C599,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C105</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C532,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C105 C38:C39 C144</xm:sqref>
+          <xm:sqref>C38:C39</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C638,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C144</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>

</xml_diff>

<commit_message>
DB - NSGs fix
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="545">
   <si>
     <t>Region</t>
   </si>
@@ -6126,7 +6126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6460,6 +6460,13 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -17717,7 +17724,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -47266,10 +47273,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -47281,11 +47288,12 @@
     <col min="5" max="5" width="23.36328125" style="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.81640625" style="37" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.1796875" style="37" customWidth="1"/>
-    <col min="8" max="18" width="8.6328125" style="37" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" style="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="18" width="8.6328125" style="37" customWidth="1"/>
     <col min="19" max="16384" width="8.6328125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="222" customHeight="1">
+    <row r="1" spans="1:8" ht="222" customHeight="1">
       <c r="A1" s="117" t="s">
         <v>431</v>
       </c>
@@ -47293,12 +47301,13 @@
       <c r="C1" s="118"/>
       <c r="D1" s="118"/>
       <c r="E1" s="118"/>
-      <c r="F1" s="117" t="s">
+      <c r="F1" s="137" t="s">
         <v>432</v>
       </c>
-      <c r="G1" s="118"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="74" t="s">
         <v>0</v>
       </c>
@@ -47320,8 +47329,11 @@
       <c r="G2" s="76" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="139" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="36"/>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -47329,8 +47341,9 @@
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="38"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -47338,8 +47351,9 @@
       <c r="E4" s="36"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="38"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="36"/>
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
@@ -47347,8 +47361,9 @@
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="38"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="36"/>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -47356,8 +47371,9 @@
       <c r="E6" s="36"/>
       <c r="F6" s="36"/>
       <c r="G6" s="36"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="38"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="36"/>
       <c r="B7" s="36"/>
       <c r="C7" s="36"/>
@@ -47365,8 +47381,9 @@
       <c r="E7" s="36"/>
       <c r="F7" s="36"/>
       <c r="G7" s="36"/>
-    </row>
-    <row r="8" spans="1:7" s="77" customFormat="1">
+      <c r="H7" s="38"/>
+    </row>
+    <row r="8" spans="1:8" s="77" customFormat="1">
       <c r="A8" s="65"/>
       <c r="B8" s="65"/>
       <c r="C8" s="65"/>
@@ -47374,8 +47391,9 @@
       <c r="E8" s="65"/>
       <c r="F8" s="65"/>
       <c r="G8" s="65"/>
-    </row>
-    <row r="9" spans="1:7" s="77" customFormat="1">
+      <c r="H8" s="46"/>
+    </row>
+    <row r="9" spans="1:8" s="77" customFormat="1">
       <c r="A9" s="65"/>
       <c r="B9" s="65"/>
       <c r="C9" s="65"/>
@@ -47383,8 +47401,9 @@
       <c r="E9" s="65"/>
       <c r="F9" s="65"/>
       <c r="G9" s="65"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="46"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="36"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -47392,8 +47411,9 @@
       <c r="E10" s="36"/>
       <c r="F10" s="36"/>
       <c r="G10" s="36"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="36"/>
       <c r="B11" s="36"/>
       <c r="C11" s="36"/>
@@ -47401,8 +47421,9 @@
       <c r="E11" s="36"/>
       <c r="F11" s="36"/>
       <c r="G11" s="36"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="36"/>
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
@@ -47410,8 +47431,9 @@
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
       <c r="G12" s="36"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="36"/>
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
@@ -47419,8 +47441,9 @@
       <c r="E13" s="36"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="38"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -47428,8 +47451,9 @@
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="38"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="36"/>
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
@@ -47437,8 +47461,9 @@
       <c r="E15" s="36"/>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="38"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="36"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
@@ -47446,8 +47471,9 @@
       <c r="E16" s="36"/>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="38"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="36"/>
       <c r="B17" s="36"/>
       <c r="C17" s="36"/>
@@ -47455,8 +47481,9 @@
       <c r="E17" s="36"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="38"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
@@ -47464,8 +47491,9 @@
       <c r="E18" s="36"/>
       <c r="F18" s="36"/>
       <c r="G18" s="36"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="38"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="36"/>
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
@@ -47473,8 +47501,9 @@
       <c r="E19" s="36"/>
       <c r="F19" s="36"/>
       <c r="G19" s="36"/>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="38"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="36"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
@@ -47482,8 +47511,9 @@
       <c r="E20" s="36"/>
       <c r="F20" s="36"/>
       <c r="G20" s="36"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="38"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="36"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -47491,8 +47521,9 @@
       <c r="E21" s="36"/>
       <c r="F21" s="36"/>
       <c r="G21" s="36"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" s="38"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="36"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -47500,8 +47531,9 @@
       <c r="E22" s="36"/>
       <c r="F22" s="36"/>
       <c r="G22" s="36"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="38"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="36"/>
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
@@ -47509,8 +47541,9 @@
       <c r="E23" s="36"/>
       <c r="F23" s="36"/>
       <c r="G23" s="36"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="38"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="36"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -47518,8 +47551,9 @@
       <c r="E24" s="36"/>
       <c r="F24" s="36"/>
       <c r="G24" s="36"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="38"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="36"/>
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
@@ -47527,8 +47561,9 @@
       <c r="E25" s="36"/>
       <c r="F25" s="36"/>
       <c r="G25" s="36"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" s="38"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -47536,8 +47571,9 @@
       <c r="E26" s="36"/>
       <c r="F26" s="36"/>
       <c r="G26" s="36"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="38"/>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="36"/>
       <c r="B27" s="36"/>
       <c r="C27" s="36"/>
@@ -47545,8 +47581,9 @@
       <c r="E27" s="36"/>
       <c r="F27" s="36"/>
       <c r="G27" s="36"/>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="38"/>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
@@ -47554,8 +47591,9 @@
       <c r="E28" s="36"/>
       <c r="F28" s="36"/>
       <c r="G28" s="36"/>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="38"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="36"/>
       <c r="B29" s="36"/>
       <c r="C29" s="36"/>
@@ -47563,8 +47601,9 @@
       <c r="E29" s="36"/>
       <c r="F29" s="36"/>
       <c r="G29" s="36"/>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="38"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="36"/>
       <c r="B30" s="36"/>
       <c r="C30" s="36"/>
@@ -47572,8 +47611,9 @@
       <c r="E30" s="36"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="38"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="36"/>
       <c r="B31" s="36"/>
       <c r="C31" s="36"/>
@@ -47581,8 +47621,9 @@
       <c r="E31" s="36"/>
       <c r="F31" s="36"/>
       <c r="G31" s="36"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="38"/>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="36"/>
       <c r="B32" s="36"/>
       <c r="C32" s="36"/>
@@ -47590,11 +47631,12 @@
       <c r="E32" s="36"/>
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
+      <c r="H32" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Added memory in gbs, boot vol size, in transit encryption to excel sheets - Instances
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrsubra/Desktop/Shruthi/cd3-automation/oci/oci_tools/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC4B01A-D8D8-DD43-907D-01269E8A8A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147FB201-35C5-164F-A921-DFE240AEBB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16540" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="553">
   <si>
     <t>Region</t>
   </si>
@@ -4276,77 +4276,6 @@
   </si>
   <si>
     <r>
-      <t>Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
-If the shape is VM.Standard.E3.Flex then specify it as VM.Standard.E3.Flex::&lt;ocpus&gt;
-"Defined Tags" -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
-                                 Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
-                               </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  Example: Operations.CostCenter=01;Users.Name=user01
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Backup Policy" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Leave it empty to not attach any backup policy to the boot volume.
-                                   Values can be either of the following: Gold | Silver | Bronze
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Custom Policy Compartment Name"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Specify the name of the compartment where the custom policy is created.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
 "Attached To Instance"  - </t>
     </r>
@@ -5598,6 +5527,192 @@
   </si>
   <si>
     <t>Reserved IPs (Y|N|OCID)</t>
+  </si>
+  <si>
+    <t>Memory In GBs</t>
+  </si>
+  <si>
+    <t>Boot Volume Size In GBs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is PV Encryption In Transit Enabled </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
+If the shape is VM.Standard.E3.Flex then specify it as VM.Standard.E3.Flex::&lt;ocpus&gt;
+Is PV Encryption In Transit Enabled </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Specify </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.Defaults to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">false </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when left empty.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"Defined Tags" -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
+                                 Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
+                               </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Example: Operations.CostCenter=01;Users.Name=user01
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Backup Policy" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Leave it empty to not attach any backup policy to the boot volume.
+                                   Values can be either of the following: Gold | Silver | Bronze
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Custom Policy Compartment Name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Specify the name of the compartment where the custom policy is created.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -9980,7 +10095,7 @@
     <row r="1" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -15150,7 +15265,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B1" s="117"/>
       <c r="C1" s="117"/>
@@ -15170,25 +15285,25 @@
         <v>6</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D2" s="32" t="s">
+        <v>423</v>
+      </c>
+      <c r="E2" s="33" t="s">
         <v>424</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>425</v>
       </c>
       <c r="F2" s="32" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>46</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J2" s="32" t="s">
         <v>272</v>
@@ -17708,10 +17823,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17725,18 +17840,18 @@
     <col min="7" max="7" width="18.1640625" style="37" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.83203125" style="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.83203125" style="37" customWidth="1"/>
-    <col min="10" max="10" width="22.1640625" style="37" customWidth="1"/>
-    <col min="11" max="11" width="26.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" style="37" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" style="37" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" customWidth="1"/>
+    <col min="10" max="13" width="22.1640625" style="37" customWidth="1"/>
+    <col min="14" max="14" width="26.83203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="37" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19" style="37" customWidth="1"/>
+    <col min="17" max="17" width="19.1640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" style="37" customWidth="1"/>
+    <col min="19" max="19" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="138" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="127" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B1" s="128"/>
       <c r="C1" s="128"/>
@@ -17746,7 +17861,7 @@
       <c r="G1" s="128"/>
       <c r="H1" s="129"/>
       <c r="I1" s="118" t="s">
-        <v>413</v>
+        <v>552</v>
       </c>
       <c r="J1" s="119"/>
       <c r="K1" s="119"/>
@@ -17754,9 +17869,12 @@
       <c r="M1" s="119"/>
       <c r="N1" s="119"/>
       <c r="O1" s="119"/>
-      <c r="P1" s="120"/>
-    </row>
-    <row r="2" spans="1:16" s="44" customFormat="1" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="120"/>
+    </row>
+    <row r="2" spans="1:19" s="44" customFormat="1" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
@@ -17788,25 +17906,34 @@
         <v>67</v>
       </c>
       <c r="K2" s="32" t="s">
+        <v>549</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>551</v>
+      </c>
+      <c r="N2" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="O2" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>412</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="Q2" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="R2" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="S2" s="32" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="38"/>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -17818,13 +17945,16 @@
       <c r="I3" s="38"/>
       <c r="J3" s="38"/>
       <c r="K3" s="38"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
       <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="36"/>
-    </row>
-    <row r="4" spans="1:16" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="36"/>
+    </row>
+    <row r="4" spans="1:19" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="24"/>
       <c r="C4" s="10"/>
@@ -17840,9 +17970,12 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
-      <c r="P4" s="38"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="38"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="38"/>
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
@@ -17859,8 +17992,11 @@
       <c r="N5" s="38"/>
       <c r="O5" s="38"/>
       <c r="P5" s="38"/>
-    </row>
-    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+    </row>
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="46"/>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
@@ -17871,14 +18007,17 @@
       <c r="H6" s="46"/>
       <c r="I6" s="38"/>
       <c r="J6" s="47"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
       <c r="N6" s="38"/>
       <c r="O6" s="38"/>
       <c r="P6" s="38"/>
-    </row>
-    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+    </row>
+    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="46"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -17889,20 +18028,23 @@
       <c r="H7" s="46"/>
       <c r="I7" s="38"/>
       <c r="J7" s="47"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
       <c r="P7" s="38"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L10" s="88"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O10" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="I1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17937,25 +18079,43 @@
           <x14:formula1>
             <xm:f>drop_down_rule_set!$S$2:$S$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L500</xm:sqref>
+          <xm:sqref>O3:O500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name." xr:uid="{00000000-0002-0000-0F00-000005000000}">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B501,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>B3 M3</xm:sqref>
+          <xm:sqref>P3 B3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name." xr:uid="{00000000-0002-0000-0F00-000007000000}">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B500,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 M4</xm:sqref>
+          <xm:sqref>P4 B4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name." xr:uid="{00000000-0002-0000-0F00-000009000000}">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B502,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B500 M5:M500</xm:sqref>
+          <xm:sqref>P5:P500 B5:B500</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0F00-00000E000000}">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_set!$T$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_set!$T$2:W501,"*?")+1,20,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>R3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0F00-00000F000000}">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_set!$T$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_set!$T$2:W500,"*?")+1,20,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>R4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0F00-000010000000}">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_set!$T$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_set!$T$2:W502,"*?")+1,20,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>R5:R500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;" xr:uid="{00000000-0002-0000-0F00-00000B000000}">
           <x14:formula1>
@@ -17974,24 +18134,6 @@
             <xm:f>INDIRECT("drop_down_rule_set!$D$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_set!$D$2:D502,"*?")+1,4,1,4))</xm:f>
           </x14:formula1>
           <xm:sqref>F5:F500</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0F00-00000E000000}">
-          <x14:formula1>
-            <xm:f>INDIRECT("drop_down_rule_set!$T$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_set!$T$2:T501,"*?")+1,20,1,4))</xm:f>
-          </x14:formula1>
-          <xm:sqref>O3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0F00-00000F000000}">
-          <x14:formula1>
-            <xm:f>INDIRECT("drop_down_rule_set!$T$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_set!$T$2:T500,"*?")+1,20,1,4))</xm:f>
-          </x14:formula1>
-          <xm:sqref>O4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0F00-000010000000}">
-          <x14:formula1>
-            <xm:f>INDIRECT("drop_down_rule_set!$T$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_set!$T$2:T502,"*?")+1,20,1,4))</xm:f>
-          </x14:formula1>
-          <xm:sqref>O5:O500</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18022,7 +18164,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="118" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
@@ -18506,13 +18648,13 @@
         <v>99</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E2" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>432</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>433</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>100</v>
@@ -18524,7 +18666,7 @@
         <v>74</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>102</v>
@@ -18912,7 +19054,7 @@
         <v>110</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G2" s="39" t="s">
         <v>111</v>
@@ -20152,7 +20294,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="52" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="118" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
@@ -20195,31 +20337,31 @@
         <v>29</v>
       </c>
       <c r="E2" s="67" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F2" s="66" t="s">
         <v>67</v>
       </c>
       <c r="G2" s="66" t="s">
+        <v>500</v>
+      </c>
+      <c r="H2" s="66" t="s">
         <v>501</v>
       </c>
-      <c r="H2" s="66" t="s">
+      <c r="I2" s="66" t="s">
         <v>502</v>
       </c>
-      <c r="I2" s="66" t="s">
+      <c r="J2" s="66" t="s">
         <v>503</v>
       </c>
-      <c r="J2" s="66" t="s">
+      <c r="K2" s="89" t="s">
         <v>504</v>
       </c>
-      <c r="K2" s="89" t="s">
+      <c r="L2" s="66" t="s">
         <v>505</v>
       </c>
-      <c r="L2" s="66" t="s">
+      <c r="M2" s="67" t="s">
         <v>506</v>
-      </c>
-      <c r="M2" s="67" t="s">
-        <v>507</v>
       </c>
       <c r="N2" s="66" t="s">
         <v>259</v>
@@ -20237,10 +20379,10 @@
         <v>262</v>
       </c>
       <c r="S2" s="66" t="s">
+        <v>507</v>
+      </c>
+      <c r="T2" s="66" t="s">
         <v>508</v>
-      </c>
-      <c r="T2" s="66" t="s">
-        <v>509</v>
       </c>
       <c r="U2" s="66" t="s">
         <v>72</v>
@@ -20252,10 +20394,10 @@
         <v>227</v>
       </c>
       <c r="X2" s="66" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Y2" s="66" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Z2" s="66" t="s">
         <v>74</v>
@@ -26481,7 +26623,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="118" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
@@ -26499,7 +26641,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D2" s="89" t="s">
         <v>66</v>
@@ -26508,10 +26650,10 @@
         <v>67</v>
       </c>
       <c r="F2" s="89" t="s">
+        <v>520</v>
+      </c>
+      <c r="G2" s="89" t="s">
         <v>521</v>
-      </c>
-      <c r="G2" s="89" t="s">
-        <v>522</v>
       </c>
       <c r="H2" s="92" t="s">
         <v>272</v>
@@ -32578,7 +32720,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="52" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="127" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B1" s="128"/>
       <c r="C1" s="128"/>
@@ -32612,46 +32754,46 @@
         <v>6</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D2" s="67" t="s">
+        <v>524</v>
+      </c>
+      <c r="E2" s="89" t="s">
         <v>525</v>
-      </c>
-      <c r="E2" s="89" t="s">
-        <v>526</v>
       </c>
       <c r="F2" s="89" t="s">
         <v>242</v>
       </c>
       <c r="G2" s="89" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H2" s="67" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I2" s="89" t="s">
         <v>259</v>
       </c>
       <c r="J2" s="89" t="s">
+        <v>526</v>
+      </c>
+      <c r="K2" s="89" t="s">
         <v>527</v>
       </c>
-      <c r="K2" s="89" t="s">
+      <c r="L2" s="89" t="s">
         <v>528</v>
-      </c>
-      <c r="L2" s="89" t="s">
-        <v>529</v>
       </c>
       <c r="M2" s="89" t="s">
         <v>72</v>
       </c>
       <c r="N2" s="89" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="O2" s="114" t="s">
         <v>74</v>
       </c>
       <c r="P2" s="114" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="Q2" s="96" t="s">
         <v>272</v>
@@ -39547,22 +39689,22 @@
   <sheetData>
     <row r="1" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C1" s="58" t="s">
         <v>266</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E1" s="49" t="s">
         <v>244</v>
       </c>
       <c r="F1" s="59" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G1" s="59" t="s">
         <v>227</v>
@@ -39571,13 +39713,13 @@
         <v>226</v>
       </c>
       <c r="I1" s="91" t="s">
+        <v>504</v>
+      </c>
+      <c r="J1" s="91" t="s">
         <v>505</v>
       </c>
-      <c r="J1" s="91" t="s">
-        <v>506</v>
-      </c>
       <c r="K1" s="59" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -39609,7 +39751,7 @@
         <v>80</v>
       </c>
       <c r="J2" s="65" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="K2" s="38">
         <v>1</v>
@@ -39617,7 +39759,7 @@
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="90" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B3" s="56" t="s">
         <v>268</v>
@@ -39644,7 +39786,7 @@
         <v>40</v>
       </c>
       <c r="J3" s="65" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K3" s="38">
         <v>2</v>
@@ -39652,7 +39794,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="90" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B4" s="38" t="s">
         <v>240</v>
@@ -39674,7 +39816,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C5" s="38" t="s">
         <v>269</v>
@@ -39694,7 +39836,7 @@
       </c>
       <c r="B6" s="38"/>
       <c r="C6" s="38" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
@@ -39707,11 +39849,11 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="90" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B7" s="38"/>
       <c r="C7" s="38" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D7" s="38"/>
       <c r="E7" s="38" t="s">
@@ -39724,11 +39866,11 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="90" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="38" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D8" s="38"/>
       <c r="E8" s="38" t="s">
@@ -39762,7 +39904,7 @@
       </c>
       <c r="B10" s="38"/>
       <c r="C10" s="38" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="38" t="s">
@@ -39775,11 +39917,11 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="90" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="38" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D11" s="38"/>
       <c r="E11" s="38" t="s">
@@ -39796,11 +39938,11 @@
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="38" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D12" s="38"/>
       <c r="E12" s="38" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F12" s="38"/>
       <c r="H12" s="38" t="s">
@@ -39813,7 +39955,7 @@
       </c>
       <c r="B13" s="38"/>
       <c r="C13" s="38" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
@@ -39828,7 +39970,7 @@
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
@@ -40362,91 +40504,91 @@
   <sheetData>
     <row r="1" spans="1:39" s="79" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1" s="87" t="s">
         <v>434</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="C1" s="87" t="s">
         <v>435</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="D1" s="87" t="s">
         <v>436</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="E1" s="87" t="s">
         <v>437</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="F1" s="87" t="s">
         <v>438</v>
-      </c>
-      <c r="F1" s="87" t="s">
-        <v>439</v>
       </c>
       <c r="G1" s="87" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="87" t="s">
+        <v>439</v>
+      </c>
+      <c r="I1" s="87" t="s">
         <v>440</v>
       </c>
-      <c r="I1" s="87" t="s">
+      <c r="J1" s="87" t="s">
         <v>441</v>
       </c>
-      <c r="J1" s="87" t="s">
+      <c r="K1" s="87" t="s">
         <v>442</v>
       </c>
-      <c r="K1" s="87" t="s">
+      <c r="L1" s="87" t="s">
         <v>443</v>
       </c>
-      <c r="L1" s="87" t="s">
+      <c r="M1" s="87" t="s">
+        <v>495</v>
+      </c>
+      <c r="N1" s="87" t="s">
         <v>444</v>
       </c>
-      <c r="M1" s="87" t="s">
+      <c r="O1" s="87" t="s">
+        <v>445</v>
+      </c>
+      <c r="P1" s="87" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q1" s="87" t="s">
+        <v>447</v>
+      </c>
+      <c r="R1" s="87" t="s">
+        <v>448</v>
+      </c>
+      <c r="S1" s="87" t="s">
+        <v>449</v>
+      </c>
+      <c r="T1" s="87" t="s">
+        <v>497</v>
+      </c>
+      <c r="U1" s="87" t="s">
+        <v>450</v>
+      </c>
+      <c r="V1" s="78" t="s">
+        <v>451</v>
+      </c>
+      <c r="W1" s="78" t="s">
+        <v>452</v>
+      </c>
+      <c r="X1" s="78" t="s">
+        <v>453</v>
+      </c>
+      <c r="Y1" s="87" t="s">
         <v>496</v>
-      </c>
-      <c r="N1" s="87" t="s">
-        <v>445</v>
-      </c>
-      <c r="O1" s="87" t="s">
-        <v>446</v>
-      </c>
-      <c r="P1" s="87" t="s">
-        <v>447</v>
-      </c>
-      <c r="Q1" s="87" t="s">
-        <v>448</v>
-      </c>
-      <c r="R1" s="87" t="s">
-        <v>449</v>
-      </c>
-      <c r="S1" s="87" t="s">
-        <v>450</v>
-      </c>
-      <c r="T1" s="87" t="s">
-        <v>498</v>
-      </c>
-      <c r="U1" s="87" t="s">
-        <v>451</v>
-      </c>
-      <c r="V1" s="78" t="s">
-        <v>452</v>
-      </c>
-      <c r="W1" s="78" t="s">
-        <v>453</v>
-      </c>
-      <c r="X1" s="78" t="s">
-        <v>454</v>
-      </c>
-      <c r="Y1" s="87" t="s">
-        <v>497</v>
       </c>
       <c r="Z1" s="78" t="s">
         <v>67</v>
       </c>
       <c r="AA1" s="78" t="s">
+        <v>454</v>
+      </c>
+      <c r="AB1" s="78" t="s">
         <v>455</v>
       </c>
-      <c r="AB1" s="78" t="s">
+      <c r="AC1" s="78" t="s">
         <v>456</v>
-      </c>
-      <c r="AC1" s="78" t="s">
-        <v>457</v>
       </c>
       <c r="AD1" s="78" t="s">
         <v>169</v>
@@ -40467,7 +40609,7 @@
         <v>174</v>
       </c>
       <c r="AJ1" s="78" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AK1" s="78" t="s">
         <v>222</v>
@@ -40499,7 +40641,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="81" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H2" s="81" t="s">
         <v>28</v>
@@ -40522,13 +40664,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="81" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="O2" s="81" t="s">
         <v>63</v>
       </c>
       <c r="P2" s="82" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="Q2" s="81" t="s">
         <v>251</v>
@@ -40548,13 +40690,13 @@
         <v>0</v>
       </c>
       <c r="V2" s="81" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="W2" s="81" t="s">
         <v>98</v>
       </c>
       <c r="X2" s="81" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Y2" s="81" t="b">
         <v>1</v>
@@ -40563,7 +40705,7 @@
         <v>108</v>
       </c>
       <c r="AA2" s="81" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AB2" s="81" t="s">
         <v>122</v>
@@ -40629,7 +40771,7 @@
         <v>42</v>
       </c>
       <c r="J3" s="81" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K3" s="81" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DHCP")&amp;":"&amp;ADDRESS(A3,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A3,4,4,1,"DHCP")))</f>
@@ -40643,7 +40785,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="81" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="O3" s="81" t="s">
         <v>253</v>
@@ -40658,7 +40800,7 @@
         <v>69</v>
       </c>
       <c r="S3" s="81" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="T3" s="81" cm="1">
         <f t="array" aca="1" ref="T3" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DedicatedVMHosts")&amp;":"&amp;ADDRESS(A3,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A3,3,4,1,"DedicatedVMHosts")))</f>
@@ -40675,7 +40817,7 @@
         <v>97</v>
       </c>
       <c r="X3" s="81" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Y3" s="81" t="b">
         <v>0</v>
@@ -40687,7 +40829,7 @@
         <v>121</v>
       </c>
       <c r="AB3" s="81" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AC3" s="81" t="s">
         <v>123</v>
@@ -40711,7 +40853,7 @@
         <v>16</v>
       </c>
       <c r="AJ3" s="81" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AK3" s="80" t="s">
         <v>225</v>
@@ -40739,7 +40881,7 @@
       </c>
       <c r="F4" s="81"/>
       <c r="G4" s="81" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H4" s="81"/>
       <c r="I4" s="81" t="s">
@@ -40769,7 +40911,7 @@
         <v>76</v>
       </c>
       <c r="S4" s="81" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="T4" s="81" cm="1">
         <f t="array" aca="1" ref="T4" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DedicatedVMHosts")&amp;":"&amp;ADDRESS(A4,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A4,3,4,1,"DedicatedVMHosts")))</f>
@@ -40782,14 +40924,14 @@
       <c r="V4" s="81"/>
       <c r="W4" s="81"/>
       <c r="X4" s="81" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Y4" s="81"/>
       <c r="Z4" s="81" t="s">
+        <v>469</v>
+      </c>
+      <c r="AA4" s="81" t="s">
         <v>470</v>
-      </c>
-      <c r="AA4" s="81" t="s">
-        <v>471</v>
       </c>
       <c r="AB4" s="81"/>
       <c r="AC4" s="81" t="s">
@@ -40836,7 +40978,7 @@
       </c>
       <c r="F5" s="81"/>
       <c r="G5" s="81" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H5" s="81"/>
       <c r="I5" s="81" t="s">
@@ -40854,7 +40996,7 @@
       </c>
       <c r="N5" s="81"/>
       <c r="O5" s="81" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="P5" s="82"/>
       <c r="Q5" s="81"/>
@@ -40871,7 +41013,7 @@
       <c r="X5" s="81"/>
       <c r="Y5" s="81"/>
       <c r="Z5" s="81" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="AA5" s="81"/>
       <c r="AB5" s="81"/>
@@ -40915,7 +41057,7 @@
       </c>
       <c r="F6" s="81"/>
       <c r="G6" s="81" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H6" s="81"/>
       <c r="I6" s="81"/>
@@ -40931,7 +41073,7 @@
       </c>
       <c r="N6" s="81"/>
       <c r="O6" s="81" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="P6" s="82"/>
       <c r="Q6" s="81"/>
@@ -40988,7 +41130,7 @@
       </c>
       <c r="F7" s="81"/>
       <c r="G7" s="81" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H7" s="81"/>
       <c r="I7" s="81"/>
@@ -41004,7 +41146,7 @@
       </c>
       <c r="N7" s="81"/>
       <c r="O7" s="81" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="P7" s="82"/>
       <c r="Q7" s="81"/>
@@ -41059,7 +41201,7 @@
       </c>
       <c r="F8" s="81"/>
       <c r="G8" s="81" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H8" s="81"/>
       <c r="I8" s="81"/>
@@ -41128,7 +41270,7 @@
       </c>
       <c r="F9" s="81"/>
       <c r="G9" s="81" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H9" s="81"/>
       <c r="I9" s="81"/>
@@ -41197,7 +41339,7 @@
       </c>
       <c r="F10" s="81"/>
       <c r="G10" s="81" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H10" s="81"/>
       <c r="I10" s="81"/>
@@ -41266,7 +41408,7 @@
       </c>
       <c r="F11" s="81"/>
       <c r="G11" s="81" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H11" s="81"/>
       <c r="I11" s="81"/>
@@ -41335,7 +41477,7 @@
       </c>
       <c r="F12" s="81"/>
       <c r="G12" s="81" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H12" s="81"/>
       <c r="I12" s="81"/>
@@ -41402,7 +41544,7 @@
       </c>
       <c r="F13" s="81"/>
       <c r="G13" s="81" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H13" s="81"/>
       <c r="I13" s="81"/>
@@ -41469,7 +41611,7 @@
       </c>
       <c r="F14" s="81"/>
       <c r="G14" s="81" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H14" s="81"/>
       <c r="I14" s="81"/>
@@ -41603,7 +41745,7 @@
       </c>
       <c r="F16" s="81"/>
       <c r="G16" s="81" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H16" s="81"/>
       <c r="I16" s="81"/>
@@ -41670,7 +41812,7 @@
       </c>
       <c r="F17" s="81"/>
       <c r="G17" s="81" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H17" s="81"/>
       <c r="I17" s="81"/>
@@ -41737,7 +41879,7 @@
       </c>
       <c r="F18" s="81"/>
       <c r="G18" s="81" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H18" s="81"/>
       <c r="I18" s="81"/>
@@ -41804,7 +41946,7 @@
       </c>
       <c r="F19" s="81"/>
       <c r="G19" s="81" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H19" s="81"/>
       <c r="I19" s="81"/>
@@ -41871,7 +42013,7 @@
       </c>
       <c r="F20" s="81"/>
       <c r="G20" s="81" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H20" s="81"/>
       <c r="I20" s="81"/>
@@ -41938,7 +42080,7 @@
       </c>
       <c r="F21" s="81"/>
       <c r="G21" s="81" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H21" s="81"/>
       <c r="I21" s="81"/>
@@ -42005,7 +42147,7 @@
       </c>
       <c r="F22" s="81"/>
       <c r="G22" s="81" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H22" s="81"/>
       <c r="I22" s="81"/>
@@ -42072,7 +42214,7 @@
       </c>
       <c r="F23" s="81"/>
       <c r="G23" s="81" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H23" s="81"/>
       <c r="I23" s="81"/>
@@ -42139,7 +42281,7 @@
       </c>
       <c r="F24" s="81"/>
       <c r="G24" s="81" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H24" s="81"/>
       <c r="I24" s="81"/>
@@ -44048,10 +44190,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="78" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B1" s="78" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -46542,7 +46684,7 @@
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C533,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C106:C107 C41:C43 C145:C146</xm:sqref>
+          <xm:sqref>C106:C107 C145:C146 C41:C43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name." xr:uid="{00000000-0002-0000-0300-00000E000000}">
           <x14:formula1>
@@ -46554,7 +46696,7 @@
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C599,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C110 C108 C149 C147</xm:sqref>
+          <xm:sqref>C110 C147 C149 C108</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name." xr:uid="{00000000-0002-0000-0300-000014000000}">
           <x14:formula1>
@@ -46566,7 +46708,7 @@
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C532,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C105 C38:C39 C144</xm:sqref>
+          <xm:sqref>C105 C144 C38:C39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name." xr:uid="{00000000-0002-0000-0300-000019000000}">
           <x14:formula1>
@@ -46628,7 +46770,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="131.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="118" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
@@ -46982,7 +47124,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="37" customFormat="1" ht="187.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="118" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
@@ -47009,7 +47151,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>12</v>
@@ -47201,14 +47343,14 @@
   <sheetData>
     <row r="1" spans="1:8" ht="222" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="118" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
       <c r="D1" s="119"/>
       <c r="E1" s="119"/>
       <c r="F1" s="124" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G1" s="125"/>
       <c r="H1" s="125"/>
@@ -47221,19 +47363,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="74" t="s">
+        <v>421</v>
+      </c>
+      <c r="D2" s="74" t="s">
         <v>422</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="E2" s="74" t="s">
         <v>423</v>
       </c>
-      <c r="E2" s="74" t="s">
+      <c r="F2" s="75" t="s">
         <v>424</v>
       </c>
-      <c r="F2" s="75" t="s">
+      <c r="G2" s="76" t="s">
         <v>425</v>
-      </c>
-      <c r="G2" s="76" t="s">
-        <v>426</v>
       </c>
       <c r="H2" s="116" t="s">
         <v>272</v>
@@ -47605,25 +47747,25 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B3" s="38"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B4" s="38"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B5" s="38"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B6" s="38"/>
     </row>

</xml_diff>

<commit_message>
modified ssh/rdp from protocol dropdown
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="553">
   <si>
     <t>Region</t>
   </si>
@@ -4465,13 +4465,7 @@
     <t>Frankfurt</t>
   </si>
   <si>
-    <t>ssh</t>
-  </si>
-  <si>
     <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>rdp</t>
   </si>
   <si>
     <t>Jeddah</t>
@@ -6563,6 +6557,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6630,9 +6627,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10095,7 +10089,7 @@
     <row r="1" spans="1:1" ht="15" thickBot="1"/>
     <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1">
       <c r="A2" s="66" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -10134,28 +10128,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="173.5" customHeight="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="117" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="124" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="125" t="s">
         <v>283</v>
       </c>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="125"/>
+      <c r="Q1" s="125"/>
+      <c r="R1" s="125"/>
     </row>
     <row r="2" spans="1:18" s="42" customFormat="1" ht="59.5" customHeight="1">
       <c r="A2" s="10" t="s">
@@ -15264,18 +15258,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>425</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
     </row>
     <row r="2" spans="1:11" ht="29" customHeight="1">
       <c r="A2" s="30" t="s">
@@ -16872,17 +16866,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="10" t="s">
@@ -16957,7 +16951,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -16973,25 +16967,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="60" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="116"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="10" t="s">
@@ -17122,28 +17116,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="118.75" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="116"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="116"/>
+      <c r="T1" s="116"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="13" t="s">
@@ -17708,15 +17702,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="72.75" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
     </row>
     <row r="2" spans="1:7" s="42" customFormat="1" ht="28.75" customHeight="1">
       <c r="A2" s="30" t="s">
@@ -17850,30 +17844,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="35" customFormat="1" ht="137" customHeight="1">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="126" t="s">
         <v>417</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="116" t="s">
-        <v>551</v>
-      </c>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="118"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="117" t="s">
+        <v>549</v>
+      </c>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="119"/>
     </row>
     <row r="2" spans="1:20" s="42" customFormat="1" ht="52.25" customHeight="1">
       <c r="A2" s="30" t="s">
@@ -17907,16 +17901,16 @@
         <v>67</v>
       </c>
       <c r="K2" s="30" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="M2" s="31" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O2" s="30" t="s">
         <v>72</v>
@@ -18167,19 +18161,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="35" customFormat="1" ht="114.75" customHeight="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="117" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="118"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="119"/>
     </row>
     <row r="2" spans="1:11" s="42" customFormat="1" ht="72.5">
       <c r="A2" s="30" t="s">
@@ -18204,7 +18198,7 @@
         <v>83</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>73</v>
@@ -18332,27 +18326,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="110.5" customHeight="1">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="129" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="131" t="s">
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="132" t="s">
         <v>290</v>
       </c>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="131"/>
-      <c r="M1" s="131"/>
-      <c r="N1" s="131"/>
-      <c r="O1" s="131"/>
-      <c r="P1" s="131"/>
-      <c r="Q1" s="131"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="132"/>
+      <c r="L1" s="132"/>
+      <c r="M1" s="132"/>
+      <c r="N1" s="132"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="51.75" customHeight="1">
       <c r="A2" s="11" t="s">
@@ -18623,27 +18617,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="35" customFormat="1" ht="122.5" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="116"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="116"/>
     </row>
     <row r="2" spans="1:19" s="35" customFormat="1" ht="43" customHeight="1">
       <c r="A2" s="19" t="s">
@@ -18656,7 +18650,7 @@
         <v>99</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>428</v>
@@ -18674,7 +18668,7 @@
         <v>74</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>102</v>
@@ -18851,13 +18845,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="42" customFormat="1" ht="108" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="30" t="s">
@@ -19021,29 +19015,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="35" customFormat="1" ht="106" customHeight="1">
-      <c r="A1" s="116" t="s">
-        <v>547</v>
-      </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="118"/>
+      <c r="A1" s="117" t="s">
+        <v>545</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="119"/>
     </row>
     <row r="2" spans="1:21" s="35" customFormat="1" ht="58.25" customHeight="1">
       <c r="A2" s="37" t="s">
@@ -19056,13 +19050,13 @@
         <v>99</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>110</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="G2" s="37" t="s">
         <v>111</v>
@@ -19279,29 +19273,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="115.75" customHeight="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="117" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="119" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="120" t="s">
         <v>298</v>
       </c>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="132"/>
-      <c r="R1" s="132"/>
-      <c r="S1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="134"/>
     </row>
     <row r="2" spans="1:19" ht="58.75" customHeight="1">
       <c r="A2" s="11" t="s">
@@ -19862,14 +19856,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="42" customFormat="1" ht="44.5" customHeight="1">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="135" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="136"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="137"/>
     </row>
     <row r="2" spans="1:6" ht="14.5" customHeight="1">
       <c r="A2" s="19" t="s">
@@ -19978,24 +19972,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="35" customFormat="1" ht="109" customHeight="1">
-      <c r="A1" s="115" t="s">
-        <v>548</v>
-      </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
+      <c r="A1" s="116" t="s">
+        <v>546</v>
+      </c>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
+      <c r="P1" s="116"/>
     </row>
     <row r="2" spans="1:16" s="35" customFormat="1" ht="46.25" customHeight="1">
       <c r="A2" s="31" t="s">
@@ -20020,7 +20014,7 @@
         <v>165</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>166</v>
@@ -20031,7 +20025,7 @@
       <c r="K2" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="L2" s="138" t="s">
+      <c r="L2" s="115" t="s">
         <v>168</v>
       </c>
       <c r="M2" s="31" t="s">
@@ -20163,17 +20157,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="114" customHeight="1">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="138" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="8" t="s">
@@ -20301,35 +20295,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="50" customFormat="1" ht="135.75" customHeight="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="117" t="s">
         <v>412</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
-      <c r="AA1" s="118"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118"/>
+      <c r="V1" s="118"/>
+      <c r="W1" s="118"/>
+      <c r="X1" s="118"/>
+      <c r="Y1" s="118"/>
+      <c r="Z1" s="118"/>
+      <c r="AA1" s="119"/>
     </row>
     <row r="2" spans="1:27" s="61" customFormat="1" ht="43.5">
       <c r="A2" s="64" t="s">
@@ -20345,31 +20339,31 @@
         <v>29</v>
       </c>
       <c r="E2" s="65" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F2" s="64" t="s">
         <v>67</v>
       </c>
       <c r="G2" s="64" t="s">
+        <v>495</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>496</v>
+      </c>
+      <c r="I2" s="64" t="s">
         <v>497</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="J2" s="64" t="s">
         <v>498</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="K2" s="87" t="s">
         <v>499</v>
       </c>
-      <c r="J2" s="64" t="s">
+      <c r="L2" s="64" t="s">
         <v>500</v>
       </c>
-      <c r="K2" s="87" t="s">
+      <c r="M2" s="65" t="s">
         <v>501</v>
-      </c>
-      <c r="L2" s="64" t="s">
-        <v>502</v>
-      </c>
-      <c r="M2" s="65" t="s">
-        <v>503</v>
       </c>
       <c r="N2" s="64" t="s">
         <v>259</v>
@@ -20387,10 +20381,10 @@
         <v>262</v>
       </c>
       <c r="S2" s="64" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="T2" s="64" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="U2" s="64" t="s">
         <v>72</v>
@@ -20402,7 +20396,7 @@
         <v>227</v>
       </c>
       <c r="X2" s="64" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="Y2" s="64" t="s">
         <v>411</v>
@@ -26630,16 +26624,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="119" customHeight="1">
-      <c r="A1" s="116" t="s">
-        <v>520</v>
-      </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
+      <c r="A1" s="117" t="s">
+        <v>518</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="1:8" ht="43.5">
       <c r="A2" s="87" t="s">
@@ -26649,7 +26643,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D2" s="87" t="s">
         <v>66</v>
@@ -26658,10 +26652,10 @@
         <v>67</v>
       </c>
       <c r="F2" s="87" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="G2" s="87" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="H2" s="90" t="s">
         <v>272</v>
@@ -32692,8 +32686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -32727,25 +32721,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="50" customFormat="1" ht="195" customHeight="1">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="126" t="s">
         <v>413</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="126"/>
-      <c r="Q1" s="126"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="127"/>
       <c r="R1" s="93"/>
       <c r="S1" s="93"/>
       <c r="T1" s="93"/>
@@ -32762,34 +32756,34 @@
         <v>6</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D2" s="65" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E2" s="87" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F2" s="87" t="s">
         <v>242</v>
       </c>
       <c r="G2" s="87" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H2" s="65" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I2" s="87" t="s">
         <v>259</v>
       </c>
       <c r="J2" s="87" t="s">
+        <v>521</v>
+      </c>
+      <c r="K2" s="87" t="s">
+        <v>522</v>
+      </c>
+      <c r="L2" s="87" t="s">
         <v>523</v>
-      </c>
-      <c r="K2" s="87" t="s">
-        <v>524</v>
-      </c>
-      <c r="L2" s="87" t="s">
-        <v>525</v>
       </c>
       <c r="M2" s="87" t="s">
         <v>72</v>
@@ -32801,7 +32795,7 @@
         <v>74</v>
       </c>
       <c r="P2" s="112" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="Q2" s="94" t="s">
         <v>272</v>
@@ -39697,22 +39691,22 @@
   <sheetData>
     <row r="1" spans="1:11" ht="43.5">
       <c r="A1" s="47" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C1" s="56" t="s">
         <v>266</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E1" s="47" t="s">
         <v>244</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>227</v>
@@ -39721,13 +39715,13 @@
         <v>226</v>
       </c>
       <c r="I1" s="89" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="J1" s="89" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K1" s="57" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16">
@@ -39759,7 +39753,7 @@
         <v>80</v>
       </c>
       <c r="J2" s="63" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="K2" s="36">
         <v>1</v>
@@ -39767,7 +39761,7 @@
     </row>
     <row r="3" spans="1:11" ht="16">
       <c r="A3" s="88" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B3" s="54" t="s">
         <v>268</v>
@@ -39794,7 +39788,7 @@
         <v>40</v>
       </c>
       <c r="J3" s="63" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="K3" s="36">
         <v>2</v>
@@ -39802,7 +39796,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="88" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>240</v>
@@ -39824,7 +39818,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C5" s="36" t="s">
         <v>269</v>
@@ -39844,7 +39838,7 @@
       </c>
       <c r="B6" s="36"/>
       <c r="C6" s="36" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="36" t="s">
@@ -39857,11 +39851,11 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="88" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B7" s="36"/>
       <c r="C7" s="36" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="36" t="s">
@@ -39874,11 +39868,11 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="88" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B8" s="36"/>
       <c r="C8" s="36" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="36" t="s">
@@ -39912,7 +39906,7 @@
       </c>
       <c r="B10" s="36"/>
       <c r="C10" s="36" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="36" t="s">
@@ -39925,11 +39919,11 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="88" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B11" s="36"/>
       <c r="C11" s="36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="36" t="s">
@@ -39946,11 +39940,11 @@
       </c>
       <c r="B12" s="36"/>
       <c r="C12" s="36" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="36" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F12" s="36"/>
       <c r="H12" s="36" t="s">
@@ -39963,7 +39957,7 @@
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="36" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
@@ -39978,7 +39972,7 @@
       </c>
       <c r="B14" s="36"/>
       <c r="C14" s="36" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
@@ -40467,8 +40461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM50"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.36328125" defaultRowHeight="14.5"/>
@@ -40548,7 +40542,7 @@
         <v>440</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>441</v>
@@ -40569,7 +40563,7 @@
         <v>446</v>
       </c>
       <c r="T1" s="85" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="U1" s="85" t="s">
         <v>447</v>
@@ -40584,7 +40578,7 @@
         <v>450</v>
       </c>
       <c r="Y1" s="85" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="Z1" s="76" t="s">
         <v>67</v>
@@ -41021,7 +41015,7 @@
       <c r="X5" s="79"/>
       <c r="Y5" s="79"/>
       <c r="Z5" s="79" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="AA5" s="79"/>
       <c r="AB5" s="79"/>
@@ -41080,9 +41074,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="79"/>
-      <c r="O6" s="79" t="s">
-        <v>471</v>
-      </c>
+      <c r="O6" s="79"/>
       <c r="P6" s="80"/>
       <c r="Q6" s="79"/>
       <c r="R6" s="79"/>
@@ -41138,7 +41130,7 @@
       </c>
       <c r="F7" s="79"/>
       <c r="G7" s="79" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H7" s="79"/>
       <c r="I7" s="79"/>
@@ -41153,9 +41145,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="79"/>
-      <c r="O7" s="79" t="s">
-        <v>473</v>
-      </c>
+      <c r="O7" s="79"/>
       <c r="P7" s="80"/>
       <c r="Q7" s="79"/>
       <c r="R7" s="79"/>
@@ -41209,7 +41199,7 @@
       </c>
       <c r="F8" s="79"/>
       <c r="G8" s="79" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H8" s="79"/>
       <c r="I8" s="79"/>
@@ -41278,7 +41268,7 @@
       </c>
       <c r="F9" s="79"/>
       <c r="G9" s="79" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H9" s="79"/>
       <c r="I9" s="79"/>
@@ -41347,7 +41337,7 @@
       </c>
       <c r="F10" s="79"/>
       <c r="G10" s="79" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H10" s="79"/>
       <c r="I10" s="79"/>
@@ -41416,7 +41406,7 @@
       </c>
       <c r="F11" s="79"/>
       <c r="G11" s="79" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H11" s="79"/>
       <c r="I11" s="79"/>
@@ -41485,7 +41475,7 @@
       </c>
       <c r="F12" s="79"/>
       <c r="G12" s="79" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H12" s="79"/>
       <c r="I12" s="79"/>
@@ -41552,7 +41542,7 @@
       </c>
       <c r="F13" s="79"/>
       <c r="G13" s="79" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H13" s="79"/>
       <c r="I13" s="79"/>
@@ -41619,7 +41609,7 @@
       </c>
       <c r="F14" s="79"/>
       <c r="G14" s="79" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H14" s="79"/>
       <c r="I14" s="79"/>
@@ -41753,7 +41743,7 @@
       </c>
       <c r="F16" s="79"/>
       <c r="G16" s="79" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H16" s="79"/>
       <c r="I16" s="79"/>
@@ -41820,7 +41810,7 @@
       </c>
       <c r="F17" s="79"/>
       <c r="G17" s="79" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H17" s="79"/>
       <c r="I17" s="79"/>
@@ -41887,7 +41877,7 @@
       </c>
       <c r="F18" s="79"/>
       <c r="G18" s="79" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H18" s="79"/>
       <c r="I18" s="79"/>
@@ -41954,7 +41944,7 @@
       </c>
       <c r="F19" s="79"/>
       <c r="G19" s="79" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="H19" s="79"/>
       <c r="I19" s="79"/>
@@ -42021,7 +42011,7 @@
       </c>
       <c r="F20" s="79"/>
       <c r="G20" s="79" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="H20" s="79"/>
       <c r="I20" s="79"/>
@@ -42088,7 +42078,7 @@
       </c>
       <c r="F21" s="79"/>
       <c r="G21" s="79" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="H21" s="79"/>
       <c r="I21" s="79"/>
@@ -42155,7 +42145,7 @@
       </c>
       <c r="F22" s="79"/>
       <c r="G22" s="79" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H22" s="79"/>
       <c r="I22" s="79"/>
@@ -42222,7 +42212,7 @@
       </c>
       <c r="F23" s="79"/>
       <c r="G23" s="79" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H23" s="79"/>
       <c r="I23" s="79"/>
@@ -42289,7 +42279,7 @@
       </c>
       <c r="F24" s="79"/>
       <c r="G24" s="79" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="H24" s="79"/>
       <c r="I24" s="79"/>
@@ -43738,13 +43728,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="42" customFormat="1" ht="105.75" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>280</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
@@ -44201,7 +44191,7 @@
         <v>430</v>
       </c>
       <c r="B1" s="76" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -44672,16 +44662,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="42" customFormat="1" ht="102.75" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>281</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
     </row>
     <row r="2" spans="1:8" s="42" customFormat="1">
       <c r="A2" s="7" t="s">
@@ -46777,20 +46767,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="131.5" customHeight="1">
-      <c r="A1" s="116" t="s">
-        <v>491</v>
-      </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="119" t="s">
+      <c r="A1" s="117" t="s">
+        <v>489</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="120" t="s">
         <v>302</v>
       </c>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="122"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="40" t="s">
@@ -47131,22 +47121,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="35" customFormat="1" ht="187.75" customHeight="1">
-      <c r="A1" s="116" t="s">
-        <v>536</v>
-      </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="116" t="s">
+      <c r="A1" s="117" t="s">
+        <v>534</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="117" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="119"/>
     </row>
     <row r="2" spans="1:12" s="42" customFormat="1" ht="45" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -47159,7 +47149,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>12</v>
@@ -47350,18 +47340,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="222" customHeight="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="117" t="s">
         <v>426</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="122" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="123" t="s">
         <v>427</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="72" t="s">
@@ -47740,10 +47730,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="42" customFormat="1" ht="94" customHeight="1">
-      <c r="A1" s="115" t="s">
-        <v>549</v>
-      </c>
-      <c r="B1" s="121"/>
+      <c r="A1" s="116" t="s">
+        <v>547</v>
+      </c>
+      <c r="B1" s="122"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
@@ -47755,19 +47745,19 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B3" s="36"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B4" s="36"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B5" s="36"/>
     </row>
@@ -47801,16 +47791,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="103.75" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
     </row>
     <row r="2" spans="1:8" s="42" customFormat="1" ht="43.25" customHeight="1">
       <c r="A2" s="10" t="s">

</xml_diff>

<commit_message>
loadbalancer logging module fix + other cosmetic chnages
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="554">
   <si>
     <t>Region</t>
   </si>
@@ -5744,6 +5744,9 @@
   </si>
   <si>
     <t>Is PV Encryption In Transit Enabled</t>
+  </si>
+  <si>
+    <t>Device</t>
   </si>
 </sst>
 </file>
@@ -17778,7 +17781,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select an OCI region">
           <x14:formula1>
             <xm:f>drop_down_rule_set!$G$2:$G$25</xm:f>
@@ -17801,7 +17804,13 @@
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B501,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:B5 B7:B499</xm:sqref>
+          <xm:sqref>B3:B5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B505,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7:B499</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
@@ -18048,7 +18057,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="14">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select an OCI region">
           <x14:formula1>
             <xm:f>drop_down_rule_set!$G$2:$G$25</xm:f>
@@ -18081,21 +18090,39 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:P501,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>P3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B501,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>P3 B3</xm:sqref>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:P500,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>P4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B500,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>P4 B4</xm:sqref>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:P502,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>P5:P500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B502,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>P5:P500 B5:B500</xm:sqref>
+          <xm:sqref>B5:B500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
@@ -18141,10 +18168,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -18155,12 +18182,13 @@
     <col min="4" max="4" width="18.453125" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.81640625" style="35" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.1796875" style="35" customWidth="1"/>
-    <col min="7" max="7" width="26.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" style="35" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" customWidth="1"/>
+    <col min="7" max="7" width="26.81640625" style="35" customWidth="1"/>
+    <col min="8" max="8" width="6.26953125" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" style="35" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="35" customFormat="1" ht="114.75" customHeight="1">
+    <row r="1" spans="1:12" s="35" customFormat="1" ht="114.75" customHeight="1">
       <c r="A1" s="117" t="s">
         <v>410</v>
       </c>
@@ -18173,9 +18201,10 @@
       <c r="H1" s="118"/>
       <c r="I1" s="118"/>
       <c r="J1" s="118"/>
-      <c r="K1" s="119"/>
-    </row>
-    <row r="2" spans="1:11" s="42" customFormat="1" ht="72.5">
+      <c r="K1" s="118"/>
+      <c r="L1" s="119"/>
+    </row>
+    <row r="2" spans="1:12" s="42" customFormat="1" ht="72.5">
       <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
@@ -18198,19 +18227,22 @@
         <v>83</v>
       </c>
       <c r="H2" s="31" t="s">
+        <v>553</v>
+      </c>
+      <c r="I2" s="31" t="s">
         <v>552</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="J2" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="K2" s="31" t="s">
         <v>409</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="L2" s="31" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="31.75" customHeight="1">
+    <row r="3" spans="1:12" ht="31.75" customHeight="1">
       <c r="A3" s="36"/>
       <c r="B3" s="34"/>
       <c r="C3" s="36"/>
@@ -18218,11 +18250,12 @@
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="36"/>
       <c r="J3" s="36"/>
-    </row>
-    <row r="4" spans="1:11" ht="31.75" customHeight="1">
+      <c r="K3" s="36"/>
+    </row>
+    <row r="4" spans="1:12" ht="31.75" customHeight="1">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -18230,11 +18263,12 @@
       <c r="E4" s="36"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
-      <c r="H4" s="44"/>
+      <c r="H4" s="34"/>
       <c r="I4" s="44"/>
-      <c r="J4" s="34"/>
-    </row>
-    <row r="5" spans="1:11" ht="28.75" customHeight="1">
+      <c r="J4" s="44"/>
+      <c r="K4" s="34"/>
+    </row>
+    <row r="5" spans="1:12" ht="28.75" customHeight="1">
       <c r="A5" s="36"/>
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
@@ -18242,19 +18276,20 @@
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
-      <c r="H5" s="44"/>
+      <c r="H5" s="36"/>
       <c r="I5" s="44"/>
-      <c r="J5" s="36"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select an OCI region">
           <x14:formula1>
             <xm:f>drop_down_rule_set!$G$2:$G$25</xm:f>
@@ -18271,19 +18306,25 @@
           <x14:formula1>
             <xm:f>drop_down_rule_set!$V$2:$V$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G500</xm:sqref>
+          <xm:sqref>G3:G500 H5:H500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>drop_down_rule_set!$S$2:$S$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H500</xm:sqref>
+          <xm:sqref>I3:I500</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:I500,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>J3:J500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B500,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:B500 I3:I500</xm:sqref>
+          <xm:sqref>B3:B500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
@@ -46635,7 +46676,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="27">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify your tenancy's Home Region for creating IAM Policies.">
           <x14:formula1>
             <xm:f>drop_down_rule_set!$G$2:$G$25</xm:f>
@@ -46668,9 +46709,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C664,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C184</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C591,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C184 C111:C142</xm:sqref>
+          <xm:sqref>C111:C142</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
@@ -46680,33 +46727,87 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C598,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C106:C107</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C533,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C106:C107 C41:C43 C145:C146</xm:sqref>
+          <xm:sqref>C41:C43</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C637,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C145:C146</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C599,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C109 C148</xm:sqref>
+          <xm:sqref>C109</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C638,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C148</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C601,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C110</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C599,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C110 C108 C149 C147</xm:sqref>
+          <xm:sqref>C108</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C640,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C149</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C638,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C147</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C599,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C104 C143</xm:sqref>
+          <xm:sqref>C104</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C638,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C143</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C599,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C105</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C532,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C105 C38:C39 C144</xm:sqref>
+          <xm:sqref>C38:C39</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C638,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>C144</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
@@ -47066,7 +47167,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify your tenancy's Home Region for creating Tags.">
           <x14:formula1>
             <xm:f>drop_down_rule_set!$G$2:$G$25</xm:f>
@@ -47081,9 +47182,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
           <x14:formula1>
-            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B500,"*?")+1,2,1,4))</xm:f>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:I500,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I500 B4:B500</xm:sqref>
+          <xm:sqref>I3:I500</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name.">
+          <x14:formula1>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:B501,"*?")+1,2,1,4))</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4:B500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name. Specify 'root' to create in root compartment.">
           <x14:formula1>

</xml_diff>

<commit_message>
CD3 Updated and Variables for custom backup policy
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrsubra/Desktop/Shruthi/cd3-automation/oci/oci_tools/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E63FF14-7A27-0E48-8956-422A8AC2B30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBBE534-E29D-F347-B3F0-DA5A62AF4EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16540" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -39747,31 +39747,31 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;" xr:uid="{00000000-0002-0000-1A00-000006000000}">
           <x14:formula1>
-            <xm:f>INDIRECT("drop_down_rule_set!$D$2:"&amp;ADDRESS(COUNTIF('/Users/shrsubra/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\shrsubra\Library\Containers\com.microsoft.Excel\Data\Documents\D:\PycharmProjects\oci_develop_new\indir\[CD3-gc35008.xlsx]drop_down_rule_set'!#REF!,"*?")+1,4,1,4))</xm:f>
+            <xm:f>INDIRECT("drop_down_rule_set!$D$2:"&amp;ADDRESS(COUNTIF('/Users/shrsubra/Library/Containers/com.microsoft.Excel/Data/Documents/Users\shrsubra\Library\Containers\com.microsoft.Excel\Data\Documents\D:\PycharmProjects\oci_develop_new\indir\[CD3-gc35008.xlsx]drop_down_rule_set'!#REF!,"*?")+1,4,1,4))</xm:f>
           </x14:formula1>
           <xm:sqref>C6:C501</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;" xr:uid="{00000000-0002-0000-1A00-000007000000}">
           <x14:formula1>
-            <xm:f>INDIRECT("drop_down_rule_set!$D$2:"&amp;ADDRESS(COUNTIF('/Users/shrsubra/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\shrsubra\Library\Containers\com.microsoft.Excel\Data\Documents\D:\PycharmProjects\oci_develop\oci_tools\cd3_automation_toolkit\example\[CD3-DRGv2-template.xlsx]drop_down_rule_set'!#REF!,"*?")+1,4,1,4))</xm:f>
+            <xm:f>INDIRECT("drop_down_rule_set!$D$2:"&amp;ADDRESS(COUNTIF('/Users/shrsubra/Library/Containers/com.microsoft.Excel/Data/Documents/Users\shrsubra\Library\Containers\com.microsoft.Excel\Data\Documents\D:\PycharmProjects\oci_develop\oci_tools\cd3_automation_toolkit\example\[CD3-DRGv2-template.xlsx]drop_down_rule_set'!#REF!,"*?")+1,4,1,4))</xm:f>
           </x14:formula1>
           <xm:sqref>E3:F1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name." xr:uid="{00000000-0002-0000-1A00-000008000000}">
           <x14:formula1>
-            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF('/Users/shrsubra/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\shrsubra\Library\Containers\com.microsoft.Excel\Data\Documents\D:\PycharmProjects\oci_develop\oci_tools\cd3_automation_toolkit\example\[CD3-DRGv2-template.xlsx]drop_down_rule_comp'!#REF!,"*?")+1,2,1,4))</xm:f>
+            <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF('/Users/shrsubra/Library/Containers/com.microsoft.Excel/Data/Documents/Users\shrsubra\Library\Containers\com.microsoft.Excel\Data\Documents\D:\PycharmProjects\oci_develop\oci_tools\cd3_automation_toolkit\example\[CD3-DRGv2-template.xlsx]drop_down_rule_comp'!#REF!,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
           <xm:sqref>B3:B1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-1A00-000009000000}">
           <x14:formula1>
-            <xm:f>'/Users/shrsubra/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\shrsubra\Library\Containers\com.microsoft.Excel\Data\Documents\D:\PycharmProjects\oci_develop_new\indir\[CD3-gc35008.xlsx]drop_down_rule_set'!#REF!</xm:f>
+            <xm:f>'/Users/shrsubra/Library/Containers/com.microsoft.Excel/Data/Documents/Users\shrsubra\Library\Containers\com.microsoft.Excel\Data\Documents\D:\PycharmProjects\oci_develop_new\indir\[CD3-gc35008.xlsx]drop_down_rule_set'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D6:D501</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select an OCI region" xr:uid="{00000000-0002-0000-1A00-00000A000000}">
           <x14:formula1>
-            <xm:f>'/Users/shrsubra/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\shrsubra\Library\Containers\com.microsoft.Excel\Data\Documents\D:\PycharmProjects\oci_develop\oci_tools\cd3_automation_toolkit\example\[CD3-DRGv2-template.xlsx]drop_down_rule_set'!#REF!</xm:f>
+            <xm:f>'/Users/shrsubra/Library/Containers/com.microsoft.Excel/Data/Documents/Users\shrsubra\Library\Containers\com.microsoft.Excel\Data\Documents\D:\PycharmProjects\oci_develop\oci_tools\cd3_automation_toolkit\example\[CD3-DRGv2-template.xlsx]drop_down_rule_set'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A1000</xm:sqref>
         </x14:dataValidation>
@@ -43830,7 +43830,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -44761,7 +44761,7 @@
   <dimension ref="A1:H195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated Tags Sheet and group desc \\ bug fix.
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrsubra/Desktop/Shruthi/cd3-automation/oci/oci_tools/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBBE534-E29D-F347-B3F0-DA5A62AF4EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BE755E-0A4A-5144-85CC-6FE49A0A0C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16540" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="554">
   <si>
     <t>Region</t>
   </si>
@@ -819,9 +819,6 @@
     <t>Validator</t>
   </si>
   <si>
-    <t>Default Tag Value</t>
-  </si>
-  <si>
     <t>Display Name</t>
   </si>
   <si>
@@ -988,9 +985,6 @@
   </si>
   <si>
     <t>Defined Tags</t>
-  </si>
-  <si>
-    <t>Default Tag Compartment</t>
   </si>
   <si>
     <t>Matching Rule</t>
@@ -3344,80 +3338,6 @@
     <t>Backend HealthCheck Interval In Millis</t>
   </si>
   <si>
-    <r>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Default Tag Compartment" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Specify the compartment to which the tag should be assigned as default.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Default Tag Value"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - To use 'User-Assigned Value':
-                                                    - Leave this field empty .
-                                         To use 'Default Values':
-                                                    - (if the Validator is set) mention one of the values in Validator.
-                                                    - (If the Validator is empty) the user can enter any value.
-Specify Tag Keys in different rows as shown in the example below.(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Example:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Tag key - 'internal' of row 5, the entries to columns till 'Namespace Description' will be automatically copied over from the row above it by the Tool Kit .</t>
-    </r>
-  </si>
-  <si>
     <t>AR8ADOS710</t>
   </si>
   <si>
@@ -5796,6 +5716,122 @@
       <t xml:space="preserve"> - Enter the OCID of  Trusted Certificate Authority</t>
     </r>
   </si>
+  <si>
+    <t>Default Tag Compartment = Default Tag Value</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Default Tag Compartment = Default Tag Value " - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Specify the compartment to which the tag should be assigned as default. Use Semi Colon as the delimeter between two values.
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:OMCDev::OMCDev-VM=${iam.principal.name};OMCDev::OMCDev-VM::demo-Application=) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Directives to specify Default Tag Value :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - To use 'User-Assigned Value':  Leave this field empty . (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: OMCDev::OMCDev-VM::demo-Application=)
+ - To use 'Default Values':
+     - (if the Validator is set) mention one of the values from Validator.
+     - (If the Validator is empty)  user can enter any value.
+Specify Tag Keys in different rows as shown in the example below.(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Tag key - 'internal' of row 5, the entries to columns till 'Namespace Description' will be automatically copied over from the row above it by the Tool Kit .</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -5804,7 +5840,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;**"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6037,6 +6073,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="11">
@@ -10174,7 +10216,7 @@
     <row r="1" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="66" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -10214,7 +10256,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="173.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
@@ -10224,7 +10266,7 @@
       <c r="G1" s="118"/>
       <c r="H1" s="119"/>
       <c r="I1" s="125" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J1" s="125"/>
       <c r="K1" s="125"/>
@@ -10289,7 +10331,7 @@
         <v>18</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="75" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15344,7 +15386,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -15364,28 +15406,28 @@
         <v>6</v>
       </c>
       <c r="C2" s="30" t="s">
+        <v>415</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="E2" s="31" t="s">
         <v>418</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>420</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>421</v>
       </c>
       <c r="F2" s="30" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="H2" s="30" t="s">
         <v>46</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K2" s="61"/>
     </row>
@@ -16952,7 +16994,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -16989,7 +17031,7 @@
         <v>47</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -17053,7 +17095,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -17122,7 +17164,7 @@
         <v>47</v>
       </c>
       <c r="Q2" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -17202,7 +17244,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="118.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -17280,10 +17322,10 @@
         <v>47</v>
       </c>
       <c r="S2" s="60" t="s">
+        <v>270</v>
+      </c>
+      <c r="T2" s="60" t="s">
         <v>271</v>
-      </c>
-      <c r="T2" s="60" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="75" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -17788,7 +17830,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -17805,7 +17847,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>66</v>
@@ -17817,7 +17859,7 @@
         <v>68</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -17930,7 +17972,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="35" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="126" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B1" s="127"/>
       <c r="C1" s="127"/>
@@ -17940,7 +17982,7 @@
       <c r="G1" s="127"/>
       <c r="H1" s="128"/>
       <c r="I1" s="117" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="J1" s="118"/>
       <c r="K1" s="118"/>
@@ -17965,7 +18007,7 @@
         <v>66</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>68</v>
@@ -17980,22 +18022,22 @@
         <v>71</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J2" s="30" t="s">
         <v>67</v>
       </c>
       <c r="K2" s="30" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="M2" s="31" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="O2" s="30" t="s">
         <v>72</v>
@@ -18004,7 +18046,7 @@
         <v>73</v>
       </c>
       <c r="Q2" s="31" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="R2" s="30" t="s">
         <v>74</v>
@@ -18013,7 +18055,7 @@
         <v>75</v>
       </c>
       <c r="T2" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -18248,7 +18290,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="35" customFormat="1" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
@@ -18285,19 +18327,19 @@
         <v>83</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="J2" s="31" t="s">
         <v>73</v>
       </c>
       <c r="K2" s="31" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18426,7 +18468,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="110.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="129" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B1" s="130"/>
       <c r="C1" s="130"/>
@@ -18436,7 +18478,7 @@
       <c r="G1" s="130"/>
       <c r="H1" s="131"/>
       <c r="I1" s="132" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J1" s="132"/>
       <c r="K1" s="132"/>
@@ -18497,7 +18539,7 @@
         <v>74</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -18717,7 +18759,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="35" customFormat="1" ht="122.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -18749,13 +18791,13 @@
         <v>99</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G2" s="19" t="s">
         <v>100</v>
@@ -18767,7 +18809,7 @@
         <v>74</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>102</v>
@@ -18788,13 +18830,13 @@
         <v>107</v>
       </c>
       <c r="Q2" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="R2" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="R2" s="19" t="s">
-        <v>258</v>
-      </c>
       <c r="S2" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -18945,7 +18987,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="42" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -18966,7 +19008,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="35" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -19115,7 +19157,7 @@
   <sheetData>
     <row r="1" spans="1:22" s="35" customFormat="1" ht="121" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
@@ -19150,16 +19192,16 @@
         <v>99</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>110</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="H2" s="37" t="s">
         <v>111</v>
@@ -19174,7 +19216,7 @@
         <v>114</v>
       </c>
       <c r="L2" s="37" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M2" s="37" t="s">
         <v>115</v>
@@ -19195,16 +19237,16 @@
         <v>120</v>
       </c>
       <c r="S2" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="T2" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="U2" s="31" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="V2" s="31" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -19381,7 +19423,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="115.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
@@ -19392,7 +19434,7 @@
       <c r="H1" s="118"/>
       <c r="I1" s="118"/>
       <c r="J1" s="120" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K1" s="133"/>
       <c r="L1" s="133"/>
@@ -19448,7 +19490,7 @@
         <v>136</v>
       </c>
       <c r="O2" s="31" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>137</v>
@@ -19964,7 +20006,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="42" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="135" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="136"/>
       <c r="C1" s="136"/>
@@ -20080,7 +20122,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="35" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -20122,16 +20164,16 @@
         <v>165</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="J2" s="31" t="s">
         <v>166</v>
       </c>
       <c r="K2" s="31" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L2" s="31" t="s">
         <v>167</v>
@@ -20140,16 +20182,16 @@
         <v>168</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O2" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="P2" s="31" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="Q2" s="31" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -20273,7 +20315,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="138" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B1" s="138"/>
       <c r="C1" s="138"/>
@@ -20292,25 +20334,25 @@
         <v>6</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="62" t="s">
         <v>218</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="F2" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>222</v>
-      </c>
       <c r="I2" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -20411,7 +20453,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="50" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
@@ -20454,73 +20496,73 @@
         <v>29</v>
       </c>
       <c r="E2" s="65" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="F2" s="64" t="s">
         <v>67</v>
       </c>
       <c r="G2" s="64" t="s">
+        <v>492</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>493</v>
+      </c>
+      <c r="I2" s="64" t="s">
+        <v>494</v>
+      </c>
+      <c r="J2" s="64" t="s">
         <v>495</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="K2" s="87" t="s">
         <v>496</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="L2" s="64" t="s">
         <v>497</v>
       </c>
-      <c r="J2" s="64" t="s">
+      <c r="M2" s="65" t="s">
         <v>498</v>
       </c>
-      <c r="K2" s="87" t="s">
+      <c r="N2" s="64" t="s">
+        <v>258</v>
+      </c>
+      <c r="O2" s="64" t="s">
+        <v>217</v>
+      </c>
+      <c r="P2" s="64" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q2" s="64" t="s">
+        <v>260</v>
+      </c>
+      <c r="R2" s="64" t="s">
+        <v>261</v>
+      </c>
+      <c r="S2" s="64" t="s">
         <v>499</v>
       </c>
-      <c r="L2" s="64" t="s">
+      <c r="T2" s="64" t="s">
         <v>500</v>
-      </c>
-      <c r="M2" s="65" t="s">
-        <v>501</v>
-      </c>
-      <c r="N2" s="64" t="s">
-        <v>259</v>
-      </c>
-      <c r="O2" s="64" t="s">
-        <v>218</v>
-      </c>
-      <c r="P2" s="64" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q2" s="64" t="s">
-        <v>261</v>
-      </c>
-      <c r="R2" s="64" t="s">
-        <v>262</v>
-      </c>
-      <c r="S2" s="64" t="s">
-        <v>502</v>
-      </c>
-      <c r="T2" s="64" t="s">
-        <v>503</v>
       </c>
       <c r="U2" s="64" t="s">
         <v>72</v>
       </c>
       <c r="V2" s="64" t="s">
+        <v>225</v>
+      </c>
+      <c r="W2" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="W2" s="64" t="s">
-        <v>227</v>
-      </c>
       <c r="X2" s="64" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="Y2" s="64" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="Z2" s="64" t="s">
         <v>74</v>
       </c>
       <c r="AA2" s="64" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
@@ -26740,7 +26782,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
@@ -26758,7 +26800,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D2" s="87" t="s">
         <v>66</v>
@@ -26767,13 +26809,13 @@
         <v>67</v>
       </c>
       <c r="F2" s="87" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="G2" s="87" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="H2" s="90" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -32837,7 +32879,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="50" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="126" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B1" s="127"/>
       <c r="C1" s="127"/>
@@ -32871,49 +32913,49 @@
         <v>6</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D2" s="65" t="s">
+        <v>516</v>
+      </c>
+      <c r="E2" s="87" t="s">
+        <v>517</v>
+      </c>
+      <c r="F2" s="87" t="s">
+        <v>241</v>
+      </c>
+      <c r="G2" s="87" t="s">
+        <v>493</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>498</v>
+      </c>
+      <c r="I2" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="J2" s="87" t="s">
+        <v>518</v>
+      </c>
+      <c r="K2" s="87" t="s">
         <v>519</v>
       </c>
-      <c r="E2" s="87" t="s">
+      <c r="L2" s="87" t="s">
         <v>520</v>
-      </c>
-      <c r="F2" s="87" t="s">
-        <v>242</v>
-      </c>
-      <c r="G2" s="87" t="s">
-        <v>496</v>
-      </c>
-      <c r="H2" s="65" t="s">
-        <v>501</v>
-      </c>
-      <c r="I2" s="87" t="s">
-        <v>259</v>
-      </c>
-      <c r="J2" s="87" t="s">
-        <v>521</v>
-      </c>
-      <c r="K2" s="87" t="s">
-        <v>522</v>
-      </c>
-      <c r="L2" s="87" t="s">
-        <v>523</v>
       </c>
       <c r="M2" s="87" t="s">
         <v>72</v>
       </c>
       <c r="N2" s="87" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="O2" s="112" t="s">
         <v>74</v>
       </c>
       <c r="P2" s="112" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="Q2" s="94" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="R2" s="46"/>
       <c r="S2" s="46"/>
@@ -39806,37 +39848,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
+        <v>507</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>494</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="56" t="s">
         <v>510</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="E1" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>498</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1" s="89" t="s">
+        <v>496</v>
+      </c>
+      <c r="J1" s="89" t="s">
         <v>497</v>
       </c>
-      <c r="C1" s="56" t="s">
-        <v>266</v>
-      </c>
-      <c r="D1" s="56" t="s">
-        <v>513</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>244</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>501</v>
-      </c>
-      <c r="G1" s="57" t="s">
-        <v>227</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>226</v>
-      </c>
-      <c r="I1" s="89" t="s">
-        <v>499</v>
-      </c>
-      <c r="J1" s="89" t="s">
-        <v>500</v>
-      </c>
       <c r="K1" s="57" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -39844,31 +39886,31 @@
         <v>78</v>
       </c>
       <c r="B2" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="51" t="s">
         <v>229</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>267</v>
-      </c>
-      <c r="D2" s="44" t="s">
+      <c r="G2" s="67" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2" s="36" t="s">
         <v>232</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>245</v>
-      </c>
-      <c r="F2" s="51" t="s">
-        <v>230</v>
-      </c>
-      <c r="G2" s="67" t="s">
-        <v>234</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>233</v>
       </c>
       <c r="I2" s="34">
         <v>80</v>
       </c>
       <c r="J2" s="63" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="K2" s="36">
         <v>1</v>
@@ -39876,34 +39918,34 @@
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="88" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B3" s="54" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F3" s="44" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G3" s="67" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I3" s="34">
         <v>40</v>
       </c>
       <c r="J3" s="63" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="K3" s="36">
         <v>2</v>
@@ -39911,659 +39953,659 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="88" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F4" s="36"/>
       <c r="H4" s="9" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="88" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F5" s="36"/>
       <c r="H5" s="36" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="88" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B6" s="36"/>
       <c r="C6" s="36" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F6" s="36"/>
       <c r="H6" s="36" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="88" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B7" s="36"/>
       <c r="C7" s="36" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="36" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F7" s="36"/>
       <c r="H7" s="36" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="88" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B8" s="36"/>
       <c r="C8" s="36" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="36" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F8" s="36"/>
       <c r="H8" s="36" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="88" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="36" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D9" s="36"/>
       <c r="E9" s="36" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F9" s="36"/>
       <c r="H9" s="36" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="88" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B10" s="36"/>
       <c r="C10" s="36" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="36" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F10" s="36"/>
       <c r="H10" s="36" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="88" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B11" s="36"/>
       <c r="C11" s="36" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="36" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F11" s="36"/>
       <c r="H11" s="36" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="88" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B12" s="36"/>
       <c r="C12" s="36" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="36" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F12" s="36"/>
       <c r="H12" s="36" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="88" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="36" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
       <c r="F13" s="36"/>
       <c r="H13" s="36" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="88" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B14" s="36"/>
       <c r="C14" s="36" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
       <c r="H14" s="36" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H15" s="36" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H16" s="36" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H17" s="36" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H18" s="36" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H19" s="36" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H20" s="36" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H21" s="36" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="22" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H22" s="36" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H23" s="36" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H24" s="36" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H25" s="36" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="26" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H26" s="36" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H27" s="36" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H28" s="36" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H29" s="36" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H30" s="36" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H31" s="36" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="32" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H32" s="36" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H33" s="36" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H34" s="36" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="35" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H35" s="36" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H36" s="36" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="37" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H37" s="36" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="38" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H38" s="36" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="39" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H39" s="36" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="40" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H40" s="36" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="41" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H41" s="36" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="42" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H42" s="36" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="43" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H43" s="36" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="44" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H44" s="36" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="45" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H45" s="36" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="46" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H46" s="36" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="47" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H47" s="36" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="48" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H48" s="36" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H49" s="36" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="50" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H50" s="36" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="51" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H51" s="36" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="52" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H52" s="36" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="53" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H53" s="36" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H54" s="36" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="55" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H55" s="36" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="56" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H56" s="36" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="57" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H57" s="36" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="58" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H58" s="36" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="59" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H59" s="36" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="60" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H60" s="36" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="61" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H61" s="36" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="62" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H62" s="36" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="63" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H63" s="36" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="64" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H64" s="36" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="65" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H65" s="36" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="66" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H66" s="36" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="67" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H67" s="36" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="68" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H68" s="36" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="69" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H69" s="36" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="70" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H70" s="36" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="71" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H71" s="36" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="72" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H72" s="36" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="73" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H73" s="36" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="74" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H74" s="36" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="75" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H75" s="36" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="76" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H76" s="36" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="77" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H77" s="36" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="78" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H78" s="36" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="79" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H79" s="36" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="80" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H80" s="36" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="81" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H81" s="36" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="82" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H82" s="36" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="83" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H83" s="36" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="84" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H84" s="36" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="85" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H85" s="36" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="86" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H86" s="36" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="87" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H87" s="36" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="88" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H88" s="36" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="89" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H89" s="36" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="90" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H90" s="36" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="91" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H91" s="36" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="92" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H92" s="36" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="93" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H93" s="36" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="94" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H94" s="36" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="95" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H95" s="36" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="96" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H96" s="36" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="97" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H97" s="36" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="98" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H98" s="36" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="99" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H99" s="36" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="100" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H100" s="36" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="101" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H101" s="36" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="102" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H102" s="36" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="103" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H103" s="36" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="104" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H104" s="36" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="105" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H105" s="36" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="106" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H106" s="36" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="107" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H107" s="36" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="108" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H108" s="36" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -40621,91 +40663,91 @@
   <sheetData>
     <row r="1" spans="1:39" s="77" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="85" t="s">
+        <v>427</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>428</v>
+      </c>
+      <c r="C1" s="85" t="s">
+        <v>429</v>
+      </c>
+      <c r="D1" s="85" t="s">
         <v>430</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="E1" s="85" t="s">
         <v>431</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="F1" s="85" t="s">
         <v>432</v>
-      </c>
-      <c r="D1" s="85" t="s">
-        <v>433</v>
-      </c>
-      <c r="E1" s="85" t="s">
-        <v>434</v>
-      </c>
-      <c r="F1" s="85" t="s">
-        <v>435</v>
       </c>
       <c r="G1" s="85" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="85" t="s">
+        <v>433</v>
+      </c>
+      <c r="I1" s="85" t="s">
+        <v>434</v>
+      </c>
+      <c r="J1" s="85" t="s">
+        <v>435</v>
+      </c>
+      <c r="K1" s="85" t="s">
         <v>436</v>
       </c>
-      <c r="I1" s="85" t="s">
+      <c r="L1" s="85" t="s">
         <v>437</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="M1" s="85" t="s">
+        <v>487</v>
+      </c>
+      <c r="N1" s="85" t="s">
         <v>438</v>
       </c>
-      <c r="K1" s="85" t="s">
+      <c r="O1" s="85" t="s">
         <v>439</v>
       </c>
-      <c r="L1" s="85" t="s">
+      <c r="P1" s="85" t="s">
         <v>440</v>
       </c>
-      <c r="M1" s="85" t="s">
-        <v>490</v>
-      </c>
-      <c r="N1" s="85" t="s">
+      <c r="Q1" s="85" t="s">
         <v>441</v>
       </c>
-      <c r="O1" s="85" t="s">
+      <c r="R1" s="85" t="s">
         <v>442</v>
       </c>
-      <c r="P1" s="85" t="s">
+      <c r="S1" s="85" t="s">
         <v>443</v>
       </c>
-      <c r="Q1" s="85" t="s">
+      <c r="T1" s="85" t="s">
+        <v>489</v>
+      </c>
+      <c r="U1" s="85" t="s">
         <v>444</v>
       </c>
-      <c r="R1" s="85" t="s">
+      <c r="V1" s="76" t="s">
         <v>445</v>
       </c>
-      <c r="S1" s="85" t="s">
+      <c r="W1" s="76" t="s">
         <v>446</v>
       </c>
-      <c r="T1" s="85" t="s">
-        <v>492</v>
-      </c>
-      <c r="U1" s="85" t="s">
+      <c r="X1" s="76" t="s">
         <v>447</v>
       </c>
-      <c r="V1" s="76" t="s">
-        <v>448</v>
-      </c>
-      <c r="W1" s="76" t="s">
-        <v>449</v>
-      </c>
-      <c r="X1" s="76" t="s">
-        <v>450</v>
-      </c>
       <c r="Y1" s="85" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="Z1" s="76" t="s">
         <v>67</v>
       </c>
       <c r="AA1" s="76" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="AB1" s="76" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="AC1" s="76" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="AD1" s="76" t="s">
         <v>169</v>
@@ -40726,10 +40768,10 @@
         <v>174</v>
       </c>
       <c r="AJ1" s="76" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="AK1" s="76" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AL1" s="76"/>
       <c r="AM1" s="76"/>
@@ -40758,7 +40800,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="79" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H2" s="79" t="s">
         <v>28</v>
@@ -40781,22 +40823,22 @@
         <v>0</v>
       </c>
       <c r="N2" s="79" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="O2" s="79" t="s">
         <v>63</v>
       </c>
       <c r="P2" s="80" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="Q2" s="79" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="R2" s="79" t="s">
         <v>42</v>
       </c>
       <c r="S2" s="79" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="T2" s="79" cm="1">
         <f t="array" aca="1" ref="T2" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DedicatedVMHosts")&amp;":"&amp;ADDRESS(A2,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A2,3,4,1,"DedicatedVMHosts")))</f>
@@ -40807,13 +40849,13 @@
         <v>0</v>
       </c>
       <c r="V2" s="79" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="W2" s="79" t="s">
         <v>98</v>
       </c>
       <c r="X2" s="79" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="Y2" s="79" t="b">
         <v>1</v>
@@ -40822,7 +40864,7 @@
         <v>108</v>
       </c>
       <c r="AA2" s="79" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="AB2" s="79" t="s">
         <v>122</v>
@@ -40852,7 +40894,7 @@
         <v>122</v>
       </c>
       <c r="AK2" s="78" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:39" s="78" customFormat="1" x14ac:dyDescent="0.2">
@@ -40879,7 +40921,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="79" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="79" t="s">
         <v>27</v>
@@ -40888,7 +40930,7 @@
         <v>42</v>
       </c>
       <c r="J3" s="79" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K3" s="79" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DHCP")&amp;":"&amp;ADDRESS(A3,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A3,4,4,1,"DHCP")))</f>
@@ -40902,10 +40944,10 @@
         <v>0</v>
       </c>
       <c r="N3" s="79" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="O3" s="79" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P3" s="80" t="s">
         <v>64</v>
@@ -40917,7 +40959,7 @@
         <v>69</v>
       </c>
       <c r="S3" s="79" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="T3" s="79" cm="1">
         <f t="array" aca="1" ref="T3" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DedicatedVMHosts")&amp;":"&amp;ADDRESS(A3,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A3,3,4,1,"DedicatedVMHosts")))</f>
@@ -40934,7 +40976,7 @@
         <v>97</v>
       </c>
       <c r="X3" s="79" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="Y3" s="79" t="b">
         <v>0</v>
@@ -40946,7 +40988,7 @@
         <v>121</v>
       </c>
       <c r="AB3" s="79" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="AC3" s="79" t="s">
         <v>123</v>
@@ -40970,10 +41012,10 @@
         <v>16</v>
       </c>
       <c r="AJ3" s="79" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="AK3" s="78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:39" s="78" customFormat="1" x14ac:dyDescent="0.2">
@@ -40998,7 +41040,7 @@
       </c>
       <c r="F4" s="79"/>
       <c r="G4" s="79" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H4" s="79"/>
       <c r="I4" s="79" t="s">
@@ -41010,7 +41052,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="79" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M4" s="79" cm="1">
         <f t="array" aca="1" ref="M4" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DRGs")&amp;":"&amp;ADDRESS(A4,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A4,3,4,1,"DRGs")))</f>
@@ -41028,7 +41070,7 @@
         <v>76</v>
       </c>
       <c r="S4" s="79" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="T4" s="79" cm="1">
         <f t="array" aca="1" ref="T4" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DedicatedVMHosts")&amp;":"&amp;ADDRESS(A4,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A4,3,4,1,"DedicatedVMHosts")))</f>
@@ -41041,14 +41083,14 @@
       <c r="V4" s="79"/>
       <c r="W4" s="79"/>
       <c r="X4" s="79" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="Y4" s="79"/>
       <c r="Z4" s="79" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="AA4" s="79" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="AB4" s="79"/>
       <c r="AC4" s="79" t="s">
@@ -41095,7 +41137,7 @@
       </c>
       <c r="F5" s="79"/>
       <c r="G5" s="79" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="H5" s="79"/>
       <c r="I5" s="79" t="s">
@@ -41113,7 +41155,7 @@
       </c>
       <c r="N5" s="79"/>
       <c r="O5" s="79" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="P5" s="80"/>
       <c r="Q5" s="79"/>
@@ -41130,7 +41172,7 @@
       <c r="X5" s="79"/>
       <c r="Y5" s="79"/>
       <c r="Z5" s="79" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="AA5" s="79"/>
       <c r="AB5" s="79"/>
@@ -41174,7 +41216,7 @@
       </c>
       <c r="F6" s="79"/>
       <c r="G6" s="79" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H6" s="79"/>
       <c r="I6" s="79"/>
@@ -41245,7 +41287,7 @@
       </c>
       <c r="F7" s="79"/>
       <c r="G7" s="79" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="H7" s="79"/>
       <c r="I7" s="79"/>
@@ -41314,7 +41356,7 @@
       </c>
       <c r="F8" s="79"/>
       <c r="G8" s="79" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="H8" s="79"/>
       <c r="I8" s="79"/>
@@ -41383,7 +41425,7 @@
       </c>
       <c r="F9" s="79"/>
       <c r="G9" s="79" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="H9" s="79"/>
       <c r="I9" s="79"/>
@@ -41452,7 +41494,7 @@
       </c>
       <c r="F10" s="79"/>
       <c r="G10" s="79" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="H10" s="79"/>
       <c r="I10" s="79"/>
@@ -41521,7 +41563,7 @@
       </c>
       <c r="F11" s="79"/>
       <c r="G11" s="79" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="H11" s="79"/>
       <c r="I11" s="79"/>
@@ -41590,7 +41632,7 @@
       </c>
       <c r="F12" s="79"/>
       <c r="G12" s="79" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="H12" s="79"/>
       <c r="I12" s="79"/>
@@ -41657,7 +41699,7 @@
       </c>
       <c r="F13" s="79"/>
       <c r="G13" s="79" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="H13" s="79"/>
       <c r="I13" s="79"/>
@@ -41724,7 +41766,7 @@
       </c>
       <c r="F14" s="79"/>
       <c r="G14" s="79" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="H14" s="79"/>
       <c r="I14" s="79"/>
@@ -41858,7 +41900,7 @@
       </c>
       <c r="F16" s="79"/>
       <c r="G16" s="79" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="H16" s="79"/>
       <c r="I16" s="79"/>
@@ -41925,7 +41967,7 @@
       </c>
       <c r="F17" s="79"/>
       <c r="G17" s="79" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="H17" s="79"/>
       <c r="I17" s="79"/>
@@ -41992,7 +42034,7 @@
       </c>
       <c r="F18" s="79"/>
       <c r="G18" s="79" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="H18" s="79"/>
       <c r="I18" s="79"/>
@@ -42059,7 +42101,7 @@
       </c>
       <c r="F19" s="79"/>
       <c r="G19" s="79" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="H19" s="79"/>
       <c r="I19" s="79"/>
@@ -42126,7 +42168,7 @@
       </c>
       <c r="F20" s="79"/>
       <c r="G20" s="79" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="H20" s="79"/>
       <c r="I20" s="79"/>
@@ -42193,7 +42235,7 @@
       </c>
       <c r="F21" s="79"/>
       <c r="G21" s="79" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="H21" s="79"/>
       <c r="I21" s="79"/>
@@ -42260,7 +42302,7 @@
       </c>
       <c r="F22" s="79"/>
       <c r="G22" s="79" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H22" s="79"/>
       <c r="I22" s="79"/>
@@ -42327,7 +42369,7 @@
       </c>
       <c r="F23" s="79"/>
       <c r="G23" s="79" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="H23" s="79"/>
       <c r="I23" s="79"/>
@@ -42394,7 +42436,7 @@
       </c>
       <c r="F24" s="79"/>
       <c r="G24" s="79" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="H24" s="79"/>
       <c r="I24" s="79"/>
@@ -43844,7 +43886,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="42" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -43862,10 +43904,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -44303,16 +44345,16 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="76" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B1" s="76" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="78"/>
       <c r="B2" s="78" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -44778,7 +44820,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="42" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -44811,7 +44853,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="69.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -46797,7 +46839,7 @@
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C533,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C106:C107 C145:C146 C41:C43</xm:sqref>
+          <xm:sqref>C106:C107 C41:C43 C145:C146</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name." xr:uid="{00000000-0002-0000-0300-00000E000000}">
           <x14:formula1>
@@ -46809,7 +46851,7 @@
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C599,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C110 C147 C149 C108</xm:sqref>
+          <xm:sqref>C110 C108 C149 C147</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name." xr:uid="{00000000-0002-0000-0300-000014000000}">
           <x14:formula1>
@@ -46821,7 +46863,7 @@
           <x14:formula1>
             <xm:f>INDIRECT("drop_down_rule_comp!$B$2:"&amp;ADDRESS(COUNTIF(drop_down_rule_comp!$B$2:C532,"*?")+1,2,1,4))</xm:f>
           </x14:formula1>
-          <xm:sqref>C105 C144 C38:C39</xm:sqref>
+          <xm:sqref>C105 C38:C39 C144</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Specify Compartment name." xr:uid="{00000000-0002-0000-0300-000019000000}">
           <x14:formula1>
@@ -46861,10 +46903,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -46877,13 +46919,12 @@
     <col min="6" max="6" width="21.83203125" style="35" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" style="35" customWidth="1"/>
     <col min="8" max="8" width="21" style="35" customWidth="1"/>
-    <col min="9" max="9" width="23.83203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="59.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="131.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="169" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
@@ -46891,13 +46932,12 @@
       <c r="E1" s="118"/>
       <c r="F1" s="119"/>
       <c r="G1" s="120" t="s">
-        <v>302</v>
+        <v>553</v>
       </c>
       <c r="H1" s="121"/>
       <c r="I1" s="121"/>
-      <c r="J1" s="122"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
@@ -46923,13 +46963,10 @@
         <v>215</v>
       </c>
       <c r="I2" s="40" t="s">
-        <v>273</v>
-      </c>
-      <c r="J2" s="40" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="104"/>
       <c r="B3" s="63"/>
       <c r="C3" s="105"/>
@@ -46939,9 +46976,8 @@
       <c r="G3" s="63"/>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-    </row>
-    <row r="4" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="104"/>
       <c r="B4" s="63"/>
       <c r="C4" s="105"/>
@@ -46951,9 +46987,8 @@
       <c r="G4" s="63"/>
       <c r="H4" s="63"/>
       <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-    </row>
-    <row r="5" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="106"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -46963,9 +46998,8 @@
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
       <c r="I5" s="107"/>
-      <c r="J5" s="106"/>
-    </row>
-    <row r="6" spans="1:10" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
@@ -46975,9 +47009,8 @@
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
       <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-    </row>
-    <row r="7" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="44"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
@@ -46987,9 +47020,8 @@
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
       <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-    </row>
-    <row r="8" spans="1:10" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -46999,9 +47031,8 @@
       <c r="G8" s="44"/>
       <c r="H8" s="44"/>
       <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-    </row>
-    <row r="9" spans="1:10" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:9" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="44"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
@@ -47011,9 +47042,8 @@
       <c r="G9" s="44"/>
       <c r="H9" s="44"/>
       <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-    </row>
-    <row r="10" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="44"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
@@ -47023,9 +47053,8 @@
       <c r="G10" s="44"/>
       <c r="H10" s="44"/>
       <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-    </row>
-    <row r="11" spans="1:10" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:9" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
@@ -47035,9 +47064,8 @@
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-    </row>
-    <row r="12" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
@@ -47047,9 +47075,8 @@
       <c r="G12" s="44"/>
       <c r="H12" s="44"/>
       <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-    </row>
-    <row r="13" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
@@ -47059,9 +47086,8 @@
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
       <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-    </row>
-    <row r="14" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="44"/>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
@@ -47071,107 +47097,87 @@
       <c r="G14" s="44"/>
       <c r="H14" s="44"/>
       <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-    </row>
-    <row r="15" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="108"/>
       <c r="I15" s="109"/>
-      <c r="J15" s="108"/>
-    </row>
-    <row r="16" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="108"/>
       <c r="I16" s="109"/>
-      <c r="J16" s="108"/>
-    </row>
-    <row r="17" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="108"/>
       <c r="I17" s="109"/>
-      <c r="J17" s="108"/>
-    </row>
-    <row r="18" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="108"/>
       <c r="I18" s="109"/>
-      <c r="J18" s="108"/>
-    </row>
-    <row r="19" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="108"/>
       <c r="I19" s="109"/>
-      <c r="J19" s="108"/>
-    </row>
-    <row r="20" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="108"/>
       <c r="I20" s="109"/>
-      <c r="J20" s="108"/>
-    </row>
-    <row r="21" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="108"/>
       <c r="I21" s="109"/>
-      <c r="J21" s="108"/>
-    </row>
-    <row r="22" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="108"/>
       <c r="I22" s="109"/>
-      <c r="J22" s="108"/>
-    </row>
-    <row r="23" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="108"/>
       <c r="I23" s="109"/>
-      <c r="J23" s="108"/>
-    </row>
-    <row r="24" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="108"/>
       <c r="I24" s="109"/>
-      <c r="J24" s="108"/>
-    </row>
-    <row r="25" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="108"/>
       <c r="I25" s="109"/>
-      <c r="J25" s="108"/>
-    </row>
-    <row r="26" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="108"/>
       <c r="I26" s="109"/>
-      <c r="J26" s="108"/>
-    </row>
-    <row r="27" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="108"/>
       <c r="I27" s="109"/>
-      <c r="J27" s="108"/>
-    </row>
-    <row r="28" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="108"/>
       <c r="I28" s="109"/>
-      <c r="J28" s="108"/>
-    </row>
-    <row r="29" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="108"/>
       <c r="I29" s="109"/>
-      <c r="J29" s="108"/>
-    </row>
-    <row r="30" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="108"/>
       <c r="I30" s="109"/>
-      <c r="J30" s="108"/>
-    </row>
-    <row r="31" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="108"/>
       <c r="I31" s="109"/>
-      <c r="J31" s="108"/>
-    </row>
-    <row r="32" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="108"/>
       <c r="I32" s="109"/>
-      <c r="J32" s="108"/>
-    </row>
-    <row r="33" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="108"/>
       <c r="I33" s="109"/>
-      <c r="J33" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This field is equivalent to specifying a list of values to Defined Tags during its creation (in OCI Console)._x000a__x000a_For entering values of type &quot;list&quot; use ENUM::&lt;values in double quotes separated by comma&gt;._x000a__x000a_For type &quot;string&quot; use ENUM::&quot;&lt;value&gt;&quot;." sqref="H4:H500" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
@@ -47237,7 +47243,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="35" customFormat="1" ht="187.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
@@ -47245,7 +47251,7 @@
       <c r="E1" s="118"/>
       <c r="F1" s="119"/>
       <c r="G1" s="117" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H1" s="118"/>
       <c r="I1" s="118"/>
@@ -47264,7 +47270,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>12</v>
@@ -47288,7 +47294,7 @@
         <v>18</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -47456,14 +47462,14 @@
   <sheetData>
     <row r="1" spans="1:8" ht="222" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
       <c r="D1" s="118"/>
       <c r="E1" s="118"/>
       <c r="F1" s="123" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G1" s="124"/>
       <c r="H1" s="124"/>
@@ -47476,22 +47482,22 @@
         <v>6</v>
       </c>
       <c r="C2" s="72" t="s">
+        <v>415</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>416</v>
+      </c>
+      <c r="E2" s="72" t="s">
+        <v>417</v>
+      </c>
+      <c r="F2" s="73" t="s">
         <v>418</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="G2" s="74" t="s">
         <v>419</v>
       </c>
-      <c r="E2" s="72" t="s">
-        <v>420</v>
-      </c>
-      <c r="F2" s="73" t="s">
-        <v>421</v>
-      </c>
-      <c r="G2" s="74" t="s">
-        <v>422</v>
-      </c>
       <c r="H2" s="114" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -47846,7 +47852,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="42" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B1" s="122"/>
     </row>
@@ -47860,19 +47866,19 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B3" s="36"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B4" s="36"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B5" s="36"/>
     </row>
@@ -47907,7 +47913,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="103.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B1" s="116"/>
       <c r="C1" s="116"/>
@@ -47940,7 +47946,7 @@
         <v>26</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="75" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Null Values Change - Tags, SecLists, Default SecLists
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrsubra/Desktop/Shruthi/cd3-automation/oci/oci_tools/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48BAAAD-F384-294F-9312-948916E0C75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9392BA03-3C34-7E4F-B7A2-79AC874C8597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16220" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,6 @@
     <externalReference r:id="rId39"/>
     <externalReference r:id="rId40"/>
     <externalReference r:id="rId41"/>
-    <externalReference r:id="rId42"/>
   </externalReferences>
   <definedNames>
     <definedName name="Action_Values" localSheetId="21">'LB Rule Set Dropdown'!$A$2:$A$12</definedName>
@@ -66,44 +65,44 @@
     <definedName name="bm_shapes_drop" localSheetId="6">[2]Database_Dropdown!$F$2:$F$3</definedName>
     <definedName name="bm_shapes_drop" localSheetId="32">[3]Database_Dropdown!$F$2:$F$3</definedName>
     <definedName name="bm_shapes_drop" localSheetId="30">[4]Database_Dropdown!$F$2:$F$3</definedName>
-    <definedName name="bm_shapes_drop" localSheetId="24">[8]Database_Dropdown!#REF!</definedName>
-    <definedName name="bm_shapes_drop" localSheetId="23">[8]Database_Dropdown!#REF!</definedName>
+    <definedName name="bm_shapes_drop" localSheetId="24">[5]Database_Dropdown!#REF!</definedName>
+    <definedName name="bm_shapes_drop" localSheetId="23">[5]Database_Dropdown!#REF!</definedName>
     <definedName name="bm_shapes_drop">Database_Dropdown!#REF!</definedName>
     <definedName name="char_set" localSheetId="10">[1]Database_Dropdown!$I$2:$I$108</definedName>
     <definedName name="char_set" localSheetId="6">[2]Database_Dropdown!$I$2:$I$108</definedName>
     <definedName name="char_set" localSheetId="32">[3]Database_Dropdown!$I$2:$I$108</definedName>
     <definedName name="char_set" localSheetId="30">[4]Database_Dropdown!$I$2:$I$108</definedName>
-    <definedName name="char_set" localSheetId="24">[8]Database_Dropdown!$H$2:$H$108</definedName>
-    <definedName name="char_set" localSheetId="23">[8]Database_Dropdown!$H$2:$H$108</definedName>
+    <definedName name="char_set" localSheetId="24">[5]Database_Dropdown!$H$2:$H$108</definedName>
+    <definedName name="char_set" localSheetId="23">[5]Database_Dropdown!$H$2:$H$108</definedName>
     <definedName name="char_set">Database_Dropdown!$H$2:$H$108</definedName>
     <definedName name="D3D1000">'DBSystems-VM-BM'!$D$3</definedName>
     <definedName name="db_sersion_drop" localSheetId="10">[1]Database_Dropdown!$C$2:$C$14</definedName>
     <definedName name="db_sersion_drop" localSheetId="6">[2]Database_Dropdown!$C$2:$C$14</definedName>
     <definedName name="db_sersion_drop" localSheetId="32">[3]Database_Dropdown!$C$2:$C$14</definedName>
     <definedName name="db_sersion_drop" localSheetId="30">[4]Database_Dropdown!$C$2:$C$14</definedName>
-    <definedName name="db_sersion_drop" localSheetId="24">[8]Database_Dropdown!$C$2:$C$14</definedName>
-    <definedName name="db_sersion_drop" localSheetId="23">[8]Database_Dropdown!$C$2:$C$14</definedName>
+    <definedName name="db_sersion_drop" localSheetId="24">[5]Database_Dropdown!$C$2:$C$14</definedName>
+    <definedName name="db_sersion_drop" localSheetId="23">[5]Database_Dropdown!$C$2:$C$14</definedName>
     <definedName name="db_sersion_drop">Database_Dropdown!$C$2:$C$14</definedName>
     <definedName name="exa_shapes_drop" localSheetId="10">[1]Database_Dropdown!$E$2:$E$11</definedName>
     <definedName name="exa_shapes_drop" localSheetId="6">[2]Database_Dropdown!$E$2:$E$11</definedName>
     <definedName name="exa_shapes_drop" localSheetId="32">[3]Database_Dropdown!$E$2:$E$11</definedName>
     <definedName name="exa_shapes_drop" localSheetId="30">[4]Database_Dropdown!$E$2:$E$11</definedName>
-    <definedName name="exa_shapes_drop" localSheetId="24">[8]Database_Dropdown!$E$2:$E$11</definedName>
-    <definedName name="exa_shapes_drop" localSheetId="23">[8]Database_Dropdown!$E$2:$E$11</definedName>
+    <definedName name="exa_shapes_drop" localSheetId="24">[5]Database_Dropdown!$E$2:$E$11</definedName>
+    <definedName name="exa_shapes_drop" localSheetId="23">[5]Database_Dropdown!$E$2:$E$11</definedName>
     <definedName name="exa_shapes_drop">Database_Dropdown!$E$2:$E$11</definedName>
     <definedName name="Header_Size" localSheetId="10">'[1]Rule Set Dropdown'!$F$2:$F$6</definedName>
     <definedName name="Header_Size" localSheetId="6">'[2]Rule Set Dropdown'!$F$2:$F$6</definedName>
     <definedName name="Header_Size" localSheetId="32">'[3]Rule Set Dropdown'!$F$2:$F$6</definedName>
     <definedName name="Header_Size" localSheetId="30">#REF!</definedName>
-    <definedName name="Header_Size" localSheetId="24">'[8]LB Rule Set Dropdown'!$F$2:$F$6</definedName>
-    <definedName name="Header_Size" localSheetId="23">'[8]LB Rule Set Dropdown'!$F$2:$F$6</definedName>
+    <definedName name="Header_Size" localSheetId="24">'[5]LB Rule Set Dropdown'!$F$2:$F$6</definedName>
+    <definedName name="Header_Size" localSheetId="23">'[5]LB Rule Set Dropdown'!$F$2:$F$6</definedName>
     <definedName name="Header_Size">'LB Rule Set Dropdown'!$F$2:$F$6</definedName>
     <definedName name="license_type_drop" localSheetId="10">[1]Database_Dropdown!$G$2:$G$3</definedName>
     <definedName name="license_type_drop" localSheetId="6">[2]Database_Dropdown!$G$2:$G$3</definedName>
     <definedName name="license_type_drop" localSheetId="32">[3]Database_Dropdown!$G$2:$G$3</definedName>
     <definedName name="license_type_drop" localSheetId="30">[4]Database_Dropdown!$G$2:$G$3</definedName>
-    <definedName name="license_type_drop" localSheetId="24">[8]Database_Dropdown!$F$2:$F$3</definedName>
-    <definedName name="license_type_drop" localSheetId="23">[8]Database_Dropdown!$F$2:$F$3</definedName>
+    <definedName name="license_type_drop" localSheetId="24">[5]Database_Dropdown!$F$2:$F$3</definedName>
+    <definedName name="license_type_drop" localSheetId="23">[5]Database_Dropdown!$F$2:$F$3</definedName>
     <definedName name="license_type_drop">Database_Dropdown!$F$2:$F$3</definedName>
     <definedName name="Match_Style" localSheetId="22">'LB Rule Set Dropdown'!$C$2:$C$6</definedName>
     <definedName name="Match_Style" localSheetId="21">'LB Rule Set Dropdown'!$C$2:$C$6</definedName>
@@ -111,15 +110,15 @@
     <definedName name="nchar_set" localSheetId="6">[2]Database_Dropdown!$H$2:$H$3</definedName>
     <definedName name="nchar_set" localSheetId="32">[3]Database_Dropdown!$H$2:$H$3</definedName>
     <definedName name="nchar_set" localSheetId="30">[4]Database_Dropdown!$H$2:$H$3</definedName>
-    <definedName name="nchar_set" localSheetId="24">[8]Database_Dropdown!$G$2:$G$3</definedName>
-    <definedName name="nchar_set" localSheetId="23">[8]Database_Dropdown!$G$2:$G$3</definedName>
+    <definedName name="nchar_set" localSheetId="24">[5]Database_Dropdown!$G$2:$G$3</definedName>
+    <definedName name="nchar_set" localSheetId="23">[5]Database_Dropdown!$G$2:$G$3</definedName>
     <definedName name="nchar_set">Database_Dropdown!$G$2:$G$3</definedName>
     <definedName name="Response_Code" localSheetId="10">'[1]Rule Set Dropdown'!$E$2:$E$7</definedName>
     <definedName name="Response_Code" localSheetId="6">'[2]Rule Set Dropdown'!$E$2:$E$7</definedName>
     <definedName name="Response_Code" localSheetId="32">'[3]Rule Set Dropdown'!$E$2:$E$7</definedName>
     <definedName name="Response_Code" localSheetId="30">#REF!</definedName>
-    <definedName name="Response_Code" localSheetId="24">'[8]LB Rule Set Dropdown'!$E$2:$E$7</definedName>
-    <definedName name="Response_Code" localSheetId="23">'[8]LB Rule Set Dropdown'!$E$2:$E$7</definedName>
+    <definedName name="Response_Code" localSheetId="24">'[5]LB Rule Set Dropdown'!$E$2:$E$7</definedName>
+    <definedName name="Response_Code" localSheetId="23">'[5]LB Rule Set Dropdown'!$E$2:$E$7</definedName>
     <definedName name="Response_Code">'LB Rule Set Dropdown'!$E$2:$E$7</definedName>
     <definedName name="Shape_Option" localSheetId="29">#REF!</definedName>
     <definedName name="Shape_Option" localSheetId="26">#REF!</definedName>
@@ -131,13 +130,13 @@
     <definedName name="Shape_Option" localSheetId="24">#REF!</definedName>
     <definedName name="Shape_Option" localSheetId="23">#REF!</definedName>
     <definedName name="Shape_Option">#REF!</definedName>
-    <definedName name="Shape_Option_DB">[5]Database!$B$10:$J$10</definedName>
+    <definedName name="Shape_Option_DB">[6]Database!$B$10:$J$10</definedName>
     <definedName name="software_drop" localSheetId="10">[1]Database_Dropdown!$B$2:$B$5</definedName>
     <definedName name="software_drop" localSheetId="6">[2]Database_Dropdown!$B$2:$B$5</definedName>
     <definedName name="software_drop" localSheetId="32">[3]Database_Dropdown!$B$2:$B$5</definedName>
     <definedName name="software_drop" localSheetId="30">[4]Database_Dropdown!$B$2:$B$5</definedName>
-    <definedName name="software_drop" localSheetId="24">[8]Database_Dropdown!$B$2:$B$5</definedName>
-    <definedName name="software_drop" localSheetId="23">[8]Database_Dropdown!$B$2:$B$5</definedName>
+    <definedName name="software_drop" localSheetId="24">[5]Database_Dropdown!$B$2:$B$5</definedName>
+    <definedName name="software_drop" localSheetId="23">[5]Database_Dropdown!$B$2:$B$5</definedName>
     <definedName name="software_drop">Database_Dropdown!$B$2:$B$5</definedName>
     <definedName name="VM_Shapes" localSheetId="29">Database_Dropdown!$A$2:$A$12</definedName>
     <definedName name="VM_Shapes" localSheetId="10">#REF!</definedName>
@@ -147,15 +146,15 @@
     <definedName name="VM_shapes_drop" localSheetId="6">[2]Database_Dropdown!$A$2:$A$7</definedName>
     <definedName name="VM_shapes_drop" localSheetId="32">[3]Database_Dropdown!$A$2:$A$7</definedName>
     <definedName name="VM_shapes_drop" localSheetId="30">[4]Database_Dropdown!$A$2:$A$7</definedName>
-    <definedName name="VM_shapes_drop" localSheetId="24">[8]Database_Dropdown!$A$2:$A$7</definedName>
-    <definedName name="VM_shapes_drop" localSheetId="23">[8]Database_Dropdown!$A$2:$A$7</definedName>
+    <definedName name="VM_shapes_drop" localSheetId="24">[5]Database_Dropdown!$A$2:$A$7</definedName>
+    <definedName name="VM_shapes_drop" localSheetId="23">[5]Database_Dropdown!$A$2:$A$7</definedName>
     <definedName name="VM_shapes_drop">Database_Dropdown!$A$2:$A$7</definedName>
     <definedName name="workload_drop" localSheetId="10">[1]Database_Dropdown!$D$2:$D$3</definedName>
     <definedName name="workload_drop" localSheetId="6">[2]Database_Dropdown!$D$2:$D$3</definedName>
     <definedName name="workload_drop" localSheetId="32">[3]Database_Dropdown!$D$2:$D$3</definedName>
     <definedName name="workload_drop" localSheetId="30">[4]Database_Dropdown!$D$2:$D$3</definedName>
-    <definedName name="workload_drop" localSheetId="24">[8]Database_Dropdown!$D$2:$D$3</definedName>
-    <definedName name="workload_drop" localSheetId="23">[8]Database_Dropdown!$D$2:$D$3</definedName>
+    <definedName name="workload_drop" localSheetId="24">[5]Database_Dropdown!$D$2:$D$3</definedName>
+    <definedName name="workload_drop" localSheetId="23">[5]Database_Dropdown!$D$2:$D$3</definedName>
     <definedName name="workload_drop">Database_Dropdown!$D$2:$D$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -5689,7 +5688,130 @@
     </r>
   </si>
   <si>
-    <t>Default Tag Compartment = Default Tag Value</t>
+    <t>SanJose</t>
+  </si>
+  <si>
+    <t>SaoPaulo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CD3 Automation Toolkit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Release - v9.2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Added Tabs for Network Load Balancers,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>modified</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tags Tab to support default tags for multiple compartments
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+</t>
+  </si>
+  <si>
+    <t>NLB Name</t>
+  </si>
+  <si>
+    <t>Is Preserve Source Destination(True|False)</t>
+  </si>
+  <si>
+    <t>Reserved IP(Y|N|OCID)</t>
+  </si>
+  <si>
+    <t>Listener Protocol(UDP|TCP|UDP/TCP|Any)</t>
+  </si>
+  <si>
+    <t>Backend Policy(FIVE_TUPLE|THREE_TUPLE|TWO_TUPLE)</t>
+  </si>
+  <si>
+    <t>Is Preserve Source(True|False)</t>
+  </si>
+  <si>
+    <t>Backend HealthCheck Protocol(HTTP|HTTPS|TCP|UDP)</t>
+  </si>
+  <si>
+    <t>Default Tag Compartment=Default Tag Value</t>
   </si>
   <si>
     <r>
@@ -5704,7 +5826,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Default Tag Compartment = Default Tag Value " - </t>
+      <t xml:space="preserve">Default Tag Compartment=Default Tag Value " - </t>
     </r>
     <r>
       <rPr>
@@ -5803,129 +5925,6 @@
       </rPr>
       <t xml:space="preserve"> Tag key - 'internal' of row 5, the entries to columns till 'Namespace Description' will be automatically copied over from the row above it by the Tool Kit .</t>
     </r>
-  </si>
-  <si>
-    <t>SanJose</t>
-  </si>
-  <si>
-    <t>SaoPaulo</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CD3 Automation Toolkit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Release - v9.2
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Added Tabs for Network Load Balancers,</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>modified</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Tags Tab to support default tags for multiple compartments
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
-</t>
-  </si>
-  <si>
-    <t>NLB Name</t>
-  </si>
-  <si>
-    <t>Is Preserve Source Destination(True|False)</t>
-  </si>
-  <si>
-    <t>Reserved IP(Y|N|OCID)</t>
-  </si>
-  <si>
-    <t>Listener Protocol(UDP|TCP|UDP/TCP|Any)</t>
-  </si>
-  <si>
-    <t>Backend Policy(FIVE_TUPLE|THREE_TUPLE|TWO_TUPLE)</t>
-  </si>
-  <si>
-    <t>Is Preserve Source(True|False)</t>
-  </si>
-  <si>
-    <t>Backend HealthCheck Protocol(HTTP|HTTPS|TCP|UDP)</t>
   </si>
 </sst>
 </file>
@@ -6745,6 +6744,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6813,12 +6818,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9868,118 +9867,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Database"/>
-      <sheetName val="Compartments"/>
-      <sheetName val="Groups"/>
-      <sheetName val="Policies"/>
-      <sheetName val="VCNs"/>
-      <sheetName val="VCN Info"/>
-      <sheetName val="Subnets"/>
-      <sheetName val="ADW_ATP"/>
-      <sheetName val="DHCP"/>
-      <sheetName val="AddRouteRules"/>
-      <sheetName val="AddSecRules"/>
-      <sheetName val="RouteRulesinOCI"/>
-      <sheetName val="SecRulesinOCI"/>
-      <sheetName val="DedicatedVMHosts"/>
-      <sheetName val="Instances"/>
-      <sheetName val="BlockVols"/>
-      <sheetName val="Tags"/>
-      <sheetName val="TagServer"/>
-      <sheetName val="TagVolume"/>
-      <sheetName val="NSGs"/>
-      <sheetName val="Sheet 2"/>
-      <sheetName val="Data_Validation Values"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>VM.Standard2.1</v>
-          </cell>
-          <cell r="C10" t="str">
-            <v>VM.Standard2.2</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>VM.Standard2.4</v>
-          </cell>
-          <cell r="E10" t="str">
-            <v>VM.Standard2.8</v>
-          </cell>
-          <cell r="G10" t="str">
-            <v>VM.Standard2.24</v>
-          </cell>
-          <cell r="H10" t="str">
-            <v>BM.DenseIO2.52</v>
-          </cell>
-          <cell r="I10" t="str">
-            <v>Exadata.Base.48</v>
-          </cell>
-          <cell r="J10" t="str">
-            <v>VM.Standard2.16</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="drop_down_rule_set"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="drop_down_rule_set"/>
-      <sheetName val="drop_down_rule_comp"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="Release-Info"/>
       <sheetName val="Compartments"/>
       <sheetName val="Groups"/>
@@ -10750,78 +10637,113 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Release-Info"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Database"/>
       <sheetName val="Compartments"/>
       <sheetName val="Groups"/>
       <sheetName val="Policies"/>
-      <sheetName val="Tags"/>
       <sheetName val="VCNs"/>
-      <sheetName val="DRGs"/>
       <sheetName val="VCN Info"/>
+      <sheetName val="Subnets"/>
+      <sheetName val="ADW_ATP"/>
       <sheetName val="DHCP"/>
-      <sheetName val="Subnets"/>
-      <sheetName val="DRGRouteRulesinOCI"/>
+      <sheetName val="AddRouteRules"/>
+      <sheetName val="AddSecRules"/>
       <sheetName val="RouteRulesinOCI"/>
       <sheetName val="SecRulesinOCI"/>
-      <sheetName val="NSGs"/>
       <sheetName val="DedicatedVMHosts"/>
       <sheetName val="Instances"/>
-      <sheetName val="BlockVolumes"/>
-      <sheetName val="FSS"/>
-      <sheetName val="LB-Hostname-Certs"/>
-      <sheetName val="BackendSet-BackendServer"/>
-      <sheetName val="LB-Listener"/>
-      <sheetName val="RuleSet"/>
-      <sheetName val="PathRouteSet"/>
-      <sheetName val="NLB-Listeners"/>
-      <sheetName val="NLB-BackendSets-BackendServers"/>
-      <sheetName val="ADW_ATP"/>
-      <sheetName val="DBSystems-VM-BM"/>
-      <sheetName val="EXA-Infra"/>
-      <sheetName val="EXA-VMClusters"/>
-      <sheetName val="Database_Dropdown"/>
+      <sheetName val="BlockVols"/>
+      <sheetName val="Tags"/>
+      <sheetName val="TagServer"/>
+      <sheetName val="TagVolume"/>
+      <sheetName val="NSGs"/>
+      <sheetName val="Sheet 2"/>
+      <sheetName val="Data_Validation Values"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>VM.Standard2.1</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v>VM.Standard2.2</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>VM.Standard2.4</v>
+          </cell>
+          <cell r="E10" t="str">
+            <v>VM.Standard2.8</v>
+          </cell>
+          <cell r="G10" t="str">
+            <v>VM.Standard2.24</v>
+          </cell>
+          <cell r="H10" t="str">
+            <v>BM.DenseIO2.52</v>
+          </cell>
+          <cell r="I10" t="str">
+            <v>Exadata.Base.48</v>
+          </cell>
+          <cell r="J10" t="str">
+            <v>VM.Standard2.16</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="drop_down_rule_set"/>
-      <sheetName val="LB Rule Set Dropdown"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="drop_down_rule_set"/>
       <sheetName val="drop_down_rule_comp"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -11164,8 +11086,8 @@
   <sheetData>
     <row r="1" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="138" t="s">
-        <v>553</v>
+      <c r="A2" s="115" t="s">
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -11204,28 +11126,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="173.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>274</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="124" t="s">
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="126" t="s">
         <v>281</v>
       </c>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
+      <c r="O1" s="126"/>
+      <c r="P1" s="126"/>
+      <c r="Q1" s="126"/>
+      <c r="R1" s="126"/>
     </row>
     <row r="2" spans="1:18" s="42" customFormat="1" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -16334,18 +16256,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>422</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
     </row>
     <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
@@ -17942,17 +17864,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -18043,25 +17965,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -18192,28 +18114,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="118.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -18778,15 +18700,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>287</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" s="42" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
@@ -18920,30 +18842,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="35" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="127" t="s">
         <v>414</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="116" t="s">
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="118" t="s">
         <v>540</v>
       </c>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="118"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="120"/>
     </row>
     <row r="2" spans="1:20" s="42" customFormat="1" ht="52.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
@@ -19238,20 +19160,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="35" customFormat="1" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="118"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="120"/>
     </row>
     <row r="2" spans="1:12" s="42" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
@@ -19416,27 +19338,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="110.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="130" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="131" t="s">
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="133" t="s">
         <v>288</v>
       </c>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="131"/>
-      <c r="M1" s="131"/>
-      <c r="N1" s="131"/>
-      <c r="O1" s="131"/>
-      <c r="P1" s="131"/>
-      <c r="Q1" s="131"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -19707,27 +19629,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="35" customFormat="1" ht="122.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
     </row>
     <row r="2" spans="1:19" s="35" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -19935,13 +19857,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="42" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
@@ -20105,30 +20027,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="35" customFormat="1" ht="121" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>547</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="118"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="120"/>
     </row>
     <row r="2" spans="1:22" s="35" customFormat="1" ht="58.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
@@ -20367,25 +20289,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="35" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>548</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
     </row>
     <row r="2" spans="1:17" s="35" customFormat="1" ht="46.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -20563,29 +20485,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="115.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="119" t="s">
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="121" t="s">
         <v>296</v>
       </c>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="132"/>
-      <c r="R1" s="132"/>
-      <c r="S1" s="133"/>
+      <c r="K1" s="134"/>
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="134"/>
+      <c r="P1" s="134"/>
+      <c r="Q1" s="134"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="135"/>
     </row>
     <row r="2" spans="1:19" ht="58.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -21146,14 +21068,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="42" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="136" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="136"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="138"/>
     </row>
     <row r="2" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -21260,25 +21182,25 @@
     <col min="8" max="9" width="8.6640625" style="35" customWidth="1"/>
     <col min="10" max="10" width="16.1640625" style="35" customWidth="1"/>
     <col min="11" max="12" width="8.6640625" style="35" customWidth="1"/>
-    <col min="13" max="18" width="8.6640625" style="139"/>
+    <col min="13" max="18" width="8.6640625" style="116"/>
     <col min="19" max="16384" width="8.6640625" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
-        <v>554</v>
-      </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="118"/>
+      <c r="A1" s="118" t="s">
+        <v>552</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="120"/>
     </row>
     <row r="2" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -21288,19 +21210,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>74</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H2" s="31" t="s">
         <v>166</v>
@@ -21309,7 +21231,7 @@
         <v>110</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="K2" s="31" t="s">
         <v>167</v>
@@ -21334,7 +21256,7 @@
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
     </row>
-    <row r="4" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
@@ -21348,7 +21270,7 @@
       <c r="K4" s="35"/>
       <c r="L4" s="35"/>
     </row>
-    <row r="5" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="35"/>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
@@ -21362,7 +21284,7 @@
       <c r="K5" s="35"/>
       <c r="L5" s="35"/>
     </row>
-    <row r="6" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
       <c r="B6" s="35"/>
       <c r="C6" s="35"/>
@@ -21376,7 +21298,7 @@
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
     </row>
-    <row r="7" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35"/>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
@@ -21390,7 +21312,7 @@
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
     </row>
-    <row r="8" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="35"/>
       <c r="B8" s="35"/>
       <c r="C8" s="35"/>
@@ -21404,7 +21326,7 @@
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
     </row>
-    <row r="9" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="35"/>
       <c r="B9" s="35"/>
       <c r="C9" s="35"/>
@@ -21418,7 +21340,7 @@
       <c r="K9" s="35"/>
       <c r="L9" s="35"/>
     </row>
-    <row r="10" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35"/>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -21432,7 +21354,7 @@
       <c r="K10" s="35"/>
       <c r="L10" s="35"/>
     </row>
-    <row r="11" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="35"/>
       <c r="B11" s="35"/>
       <c r="C11" s="35"/>
@@ -21446,7 +21368,7 @@
       <c r="K11" s="35"/>
       <c r="L11" s="35"/>
     </row>
-    <row r="12" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="35"/>
       <c r="B12" s="35"/>
       <c r="C12" s="35"/>
@@ -21460,7 +21382,7 @@
       <c r="K12" s="35"/>
       <c r="L12" s="35"/>
     </row>
-    <row r="13" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="35"/>
       <c r="B13" s="35"/>
       <c r="C13" s="35"/>
@@ -21474,7 +21396,7 @@
       <c r="K13" s="35"/>
       <c r="L13" s="35"/>
     </row>
-    <row r="14" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="35"/>
       <c r="B14" s="35"/>
       <c r="C14" s="35"/>
@@ -21488,7 +21410,7 @@
       <c r="K14" s="35"/>
       <c r="L14" s="35"/>
     </row>
-    <row r="15" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35"/>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
@@ -21502,7 +21424,7 @@
       <c r="K15" s="35"/>
       <c r="L15" s="35"/>
     </row>
-    <row r="16" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="35"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
@@ -21516,7 +21438,7 @@
       <c r="K16" s="35"/>
       <c r="L16" s="35"/>
     </row>
-    <row r="17" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="35"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -21530,7 +21452,7 @@
       <c r="K17" s="35"/>
       <c r="L17" s="35"/>
     </row>
-    <row r="18" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="35"/>
       <c r="B18" s="35"/>
       <c r="C18" s="35"/>
@@ -21544,7 +21466,7 @@
       <c r="K18" s="35"/>
       <c r="L18" s="35"/>
     </row>
-    <row r="19" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="35"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
@@ -21558,7 +21480,7 @@
       <c r="K19" s="35"/>
       <c r="L19" s="35"/>
     </row>
-    <row r="20" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="35"/>
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
@@ -21572,7 +21494,7 @@
       <c r="K20" s="35"/>
       <c r="L20" s="35"/>
     </row>
-    <row r="21" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="35"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -21586,7 +21508,7 @@
       <c r="K21" s="35"/>
       <c r="L21" s="35"/>
     </row>
-    <row r="22" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="35"/>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
@@ -21600,7 +21522,7 @@
       <c r="K22" s="35"/>
       <c r="L22" s="35"/>
     </row>
-    <row r="23" spans="1:12" s="139" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="35"/>
       <c r="B23" s="35"/>
       <c r="C23" s="35"/>
@@ -21646,19 +21568,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
-        <v>554</v>
-      </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
+      <c r="A1" s="118" t="s">
+        <v>552</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
     </row>
     <row r="2" spans="1:11" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -21668,19 +21590,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>558</v>
+      </c>
+      <c r="G2" s="31" t="s">
         <v>559</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>560</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>561</v>
       </c>
       <c r="H2" s="31" t="s">
         <v>113</v>
@@ -21741,17 +21663,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="139" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
@@ -21879,35 +21801,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="50" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>409</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
-      <c r="AA1" s="118"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="119"/>
+      <c r="Y1" s="119"/>
+      <c r="Z1" s="119"/>
+      <c r="AA1" s="120"/>
     </row>
     <row r="2" spans="1:27" s="61" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
@@ -28208,16 +28130,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="119" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>513</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
     </row>
     <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="86" t="s">
@@ -34305,25 +34227,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="50" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="127" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="126"/>
-      <c r="Q1" s="126"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
+      <c r="P1" s="128"/>
+      <c r="Q1" s="128"/>
       <c r="R1" s="92"/>
       <c r="S1" s="92"/>
       <c r="T1" s="92"/>
@@ -41268,13 +41190,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="42" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -43463,7 +43385,7 @@
       </c>
       <c r="F16" s="78"/>
       <c r="G16" s="78" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="H16" s="78"/>
       <c r="I16" s="78"/>
@@ -43597,7 +43519,7 @@
       </c>
       <c r="F18" s="78"/>
       <c r="G18" s="78" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="H18" s="78"/>
       <c r="I18" s="78"/>
@@ -46246,16 +46168,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="42" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
     </row>
     <row r="2" spans="1:8" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -48333,7 +48255,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -48350,19 +48272,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="169" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>484</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="119" t="s">
-        <v>550</v>
-      </c>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="121" t="s">
+        <v>561</v>
+      </c>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
@@ -48390,7 +48312,7 @@
         <v>215</v>
       </c>
       <c r="I2" s="40" t="s">
-        <v>549</v>
+        <v>560</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="74" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48669,22 +48591,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="35" customFormat="1" ht="187.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>529</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="116" t="s">
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="118" t="s">
         <v>289</v>
       </c>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="118"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="120"/>
     </row>
     <row r="2" spans="1:12" s="42" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
@@ -48888,18 +48810,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="222" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>423</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="121" t="s">
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="123" t="s">
         <v>424</v>
       </c>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="71" t="s">
@@ -49278,10 +49200,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="42" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="123"/>
+      <c r="B1" s="125"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -49339,16 +49261,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="103.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>280</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
     </row>
     <row r="2" spans="1:8" s="42" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">

</xml_diff>

<commit_message>
network.md and excel sheets CPU Core Count
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrsubra/Desktop/Shruthi/cd3-automation/oci/oci_tools/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA30B82-0D7B-7E42-94F9-67A3A63E2095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA856E9-3FA5-F84B-A1F4-432EE88715BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16220" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,6 @@
     <externalReference r:id="rId39"/>
     <externalReference r:id="rId40"/>
     <externalReference r:id="rId41"/>
-    <externalReference r:id="rId42"/>
   </externalReferences>
   <definedNames>
     <definedName name="Action_Values" localSheetId="21">'LB Rule Set Dropdown'!$A$2:$A$12</definedName>
@@ -197,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="567">
   <si>
     <t>Region</t>
   </si>
@@ -854,9 +853,6 @@
   </si>
   <si>
     <t>Admin Password</t>
-  </si>
-  <si>
-    <t>CPU Count</t>
   </si>
   <si>
     <t>ADW or ATP</t>
@@ -10860,83 +10856,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Release-Info"/>
-      <sheetName val="Compartments"/>
-      <sheetName val="Groups"/>
-      <sheetName val="Policies"/>
-      <sheetName val="Tags"/>
-      <sheetName val="VCNs"/>
-      <sheetName val="DRGs"/>
-      <sheetName val="VCN Info"/>
-      <sheetName val="DHCP"/>
-      <sheetName val="Subnets"/>
-      <sheetName val="DRGRouteRulesinOCI"/>
-      <sheetName val="RouteRulesinOCI"/>
-      <sheetName val="SecRulesinOCI"/>
-      <sheetName val="NSGs"/>
-      <sheetName val="DedicatedVMHosts"/>
-      <sheetName val="Instances"/>
-      <sheetName val="BlockVolumes"/>
-      <sheetName val="FSS"/>
-      <sheetName val="LB-Hostname-Certs"/>
-      <sheetName val="BackendSet-BackendServer"/>
-      <sheetName val="LB-Listener"/>
-      <sheetName val="RuleSet"/>
-      <sheetName val="PathRouteSet"/>
-      <sheetName val="NLB-Listeners"/>
-      <sheetName val="NLB-BackendSets-BackendServers"/>
-      <sheetName val="ADB"/>
-      <sheetName val="DBSystems-VM-BM"/>
-      <sheetName val="EXA-Infra"/>
-      <sheetName val="EXA-VMClusters"/>
-      <sheetName val="Database_Dropdown"/>
-      <sheetName val="drop_down_rule_set"/>
-      <sheetName val="LB Rule Set Dropdown"/>
-      <sheetName val="drop_down_rule_comp"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11275,7 +11194,7 @@
     <row r="1" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -11315,7 +11234,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="173.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -11325,7 +11244,7 @@
       <c r="G1" s="82"/>
       <c r="H1" s="83"/>
       <c r="I1" s="88" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J1" s="88"/>
       <c r="K1" s="88"/>
@@ -11390,7 +11309,7 @@
         <v>18</v>
       </c>
       <c r="R2" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="52" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -16102,7 +16021,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -16122,28 +16041,28 @@
         <v>6</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D2" s="28" t="s">
+        <v>414</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>415</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>416</v>
       </c>
       <c r="F2" s="28" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>46</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K2" s="48"/>
     </row>
@@ -16202,7 +16121,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -16239,7 +16158,7 @@
         <v>47</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -16303,7 +16222,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -16372,7 +16291,7 @@
         <v>47</v>
       </c>
       <c r="Q2" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -16452,7 +16371,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="125" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -16530,10 +16449,10 @@
         <v>47</v>
       </c>
       <c r="S2" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="T2" s="47" t="s">
         <v>269</v>
-      </c>
-      <c r="T2" s="47" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -16628,7 +16547,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -16657,7 +16576,7 @@
         <v>68</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -16728,7 +16647,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="31" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B1" s="90"/>
       <c r="C1" s="90"/>
@@ -16738,7 +16657,7 @@
       <c r="G1" s="90"/>
       <c r="H1" s="91"/>
       <c r="I1" s="81" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J1" s="82"/>
       <c r="K1" s="82"/>
@@ -16778,22 +16697,22 @@
         <v>71</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>67</v>
       </c>
       <c r="K2" s="28" t="s">
+        <v>530</v>
+      </c>
+      <c r="L2" s="28" t="s">
         <v>531</v>
       </c>
-      <c r="L2" s="28" t="s">
-        <v>532</v>
-      </c>
       <c r="M2" s="29" t="s">
+        <v>535</v>
+      </c>
+      <c r="N2" s="29" t="s">
         <v>536</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>537</v>
       </c>
       <c r="O2" s="28" t="s">
         <v>72</v>
@@ -16802,7 +16721,7 @@
         <v>73</v>
       </c>
       <c r="Q2" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="R2" s="28" t="s">
         <v>74</v>
@@ -16811,7 +16730,7 @@
         <v>75</v>
       </c>
       <c r="T2" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -16905,7 +16824,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="31" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -16942,19 +16861,19 @@
         <v>83</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J2" s="29" t="s">
         <v>73</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -17044,7 +16963,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="110.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="92" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B1" s="93"/>
       <c r="C1" s="93"/>
@@ -17054,7 +16973,7 @@
       <c r="G1" s="93"/>
       <c r="H1" s="94"/>
       <c r="I1" s="95" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J1" s="95"/>
       <c r="K1" s="95"/>
@@ -17115,7 +17034,7 @@
         <v>74</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -17184,7 +17103,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="31" customFormat="1" ht="122.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -17216,13 +17135,13 @@
         <v>99</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>419</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>420</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>421</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>100</v>
@@ -17234,7 +17153,7 @@
         <v>74</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>102</v>
@@ -17255,13 +17174,13 @@
         <v>107</v>
       </c>
       <c r="Q2" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="R2" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="R2" s="18" t="s">
-        <v>256</v>
-      </c>
       <c r="S2" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -17328,7 +17247,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="37" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -17349,7 +17268,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -17407,7 +17326,7 @@
   <sheetData>
     <row r="1" spans="1:22" s="31" customFormat="1" ht="121" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -17442,16 +17361,16 @@
         <v>99</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>110</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H2" s="33" t="s">
         <v>111</v>
@@ -17466,7 +17385,7 @@
         <v>114</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M2" s="33" t="s">
         <v>115</v>
@@ -17487,16 +17406,16 @@
         <v>120</v>
       </c>
       <c r="S2" s="29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T2" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U2" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="V2" s="29" t="s">
         <v>295</v>
-      </c>
-      <c r="V2" s="29" t="s">
-        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -17573,7 +17492,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="31" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -17615,16 +17534,16 @@
         <v>165</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J2" s="29" t="s">
         <v>166</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L2" s="29" t="s">
         <v>167</v>
@@ -17633,16 +17552,16 @@
         <v>168</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P2" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q2" s="29" t="s">
         <v>295</v>
-      </c>
-      <c r="Q2" s="29" t="s">
-        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -17693,7 +17612,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -17704,7 +17623,7 @@
       <c r="H1" s="82"/>
       <c r="I1" s="82"/>
       <c r="J1" s="84" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K1" s="96"/>
       <c r="L1" s="96"/>
@@ -17760,7 +17679,7 @@
         <v>136</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>137</v>
@@ -17835,7 +17754,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="37" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="98" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -17914,7 +17833,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -17936,19 +17855,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>74</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>166</v>
@@ -17957,13 +17876,13 @@
         <v>110</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="K2" s="29" t="s">
         <v>167</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -18295,7 +18214,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -18316,19 +18235,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="29" t="s">
+        <v>550</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>551</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="G2" s="29" t="s">
         <v>552</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>553</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>113</v>
@@ -18337,10 +18256,10 @@
         <v>114</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -18394,7 +18313,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="160" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -18420,46 +18339,46 @@
         <v>6</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>217</v>
       </c>
       <c r="G2" s="49" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H2" s="79" t="s">
         <v>218</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>219</v>
+        <v>485</v>
       </c>
       <c r="J2" s="18" t="s">
+        <v>562</v>
+      </c>
+      <c r="K2" s="18" t="s">
         <v>563</v>
       </c>
-      <c r="K2" s="18" t="s">
-        <v>564</v>
-      </c>
       <c r="L2" s="50" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="M2" s="49" t="s">
+        <v>223</v>
+      </c>
+      <c r="N2" s="49" t="s">
         <v>224</v>
-      </c>
-      <c r="N2" s="49" t="s">
-        <v>225</v>
       </c>
       <c r="O2" s="49" t="s">
         <v>74</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -18553,7 +18472,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="41" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -18596,73 +18515,73 @@
         <v>29</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F2" s="49" t="s">
         <v>67</v>
       </c>
       <c r="G2" s="49" t="s">
+        <v>484</v>
+      </c>
+      <c r="H2" s="49" t="s">
         <v>485</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="I2" s="49" t="s">
         <v>486</v>
       </c>
-      <c r="I2" s="49" t="s">
+      <c r="J2" s="49" t="s">
         <v>487</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="K2" s="64" t="s">
         <v>488</v>
       </c>
-      <c r="K2" s="64" t="s">
+      <c r="L2" s="49" t="s">
         <v>489</v>
       </c>
-      <c r="L2" s="49" t="s">
+      <c r="M2" s="50" t="s">
         <v>490</v>
       </c>
-      <c r="M2" s="50" t="s">
-        <v>491</v>
-      </c>
       <c r="N2" s="49" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O2" s="49" t="s">
         <v>217</v>
       </c>
       <c r="P2" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q2" s="49" t="s">
         <v>258</v>
       </c>
-      <c r="Q2" s="49" t="s">
+      <c r="R2" s="49" t="s">
         <v>259</v>
       </c>
-      <c r="R2" s="49" t="s">
-        <v>260</v>
-      </c>
       <c r="S2" s="49" t="s">
+        <v>491</v>
+      </c>
+      <c r="T2" s="49" t="s">
         <v>492</v>
-      </c>
-      <c r="T2" s="49" t="s">
-        <v>493</v>
       </c>
       <c r="U2" s="49" t="s">
         <v>72</v>
       </c>
       <c r="V2" s="49" t="s">
+        <v>223</v>
+      </c>
+      <c r="W2" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="W2" s="49" t="s">
-        <v>225</v>
-      </c>
       <c r="X2" s="49" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Y2" s="49" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Z2" s="49" t="s">
         <v>74</v>
       </c>
       <c r="AA2" s="49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
@@ -24698,7 +24617,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -24716,7 +24635,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D2" s="64" t="s">
         <v>66</v>
@@ -24725,13 +24644,13 @@
         <v>67</v>
       </c>
       <c r="F2" s="64" t="s">
+        <v>504</v>
+      </c>
+      <c r="G2" s="64" t="s">
         <v>505</v>
       </c>
-      <c r="G2" s="64" t="s">
-        <v>506</v>
-      </c>
       <c r="H2" s="67" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -30768,7 +30687,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="41" customFormat="1" ht="200" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B1" s="90"/>
       <c r="C1" s="90"/>
@@ -30802,49 +30721,49 @@
         <v>6</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D2" s="50" t="s">
+        <v>508</v>
+      </c>
+      <c r="E2" s="64" t="s">
         <v>509</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="F2" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>485</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>490</v>
+      </c>
+      <c r="I2" s="64" t="s">
+        <v>256</v>
+      </c>
+      <c r="J2" s="64" t="s">
         <v>510</v>
       </c>
-      <c r="F2" s="64" t="s">
-        <v>240</v>
-      </c>
-      <c r="G2" s="64" t="s">
-        <v>486</v>
-      </c>
-      <c r="H2" s="50" t="s">
-        <v>491</v>
-      </c>
-      <c r="I2" s="64" t="s">
-        <v>257</v>
-      </c>
-      <c r="J2" s="64" t="s">
+      <c r="K2" s="64" t="s">
         <v>511</v>
       </c>
-      <c r="K2" s="64" t="s">
+      <c r="L2" s="64" t="s">
         <v>512</v>
-      </c>
-      <c r="L2" s="64" t="s">
-        <v>513</v>
       </c>
       <c r="M2" s="64" t="s">
         <v>72</v>
       </c>
       <c r="N2" s="64" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="O2" s="74" t="s">
         <v>74</v>
       </c>
       <c r="P2" s="74" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="Q2" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R2" s="39"/>
       <c r="S2" s="39"/>
@@ -37662,7 +37581,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="37" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -37680,10 +37599,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -37738,40 +37657,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H1" s="46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I1" s="66" t="s">
+        <v>488</v>
+      </c>
+      <c r="J1" s="66" t="s">
         <v>489</v>
       </c>
-      <c r="J1" s="66" t="s">
-        <v>490</v>
-      </c>
       <c r="K1" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L1" s="45" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -37779,738 +37698,738 @@
         <v>78</v>
       </c>
       <c r="B2" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="42" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="D2" s="32" t="s">
+      <c r="G2" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="H2" s="32" t="s">
         <v>230</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>243</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>228</v>
-      </c>
-      <c r="G2" s="51" t="s">
-        <v>232</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>231</v>
       </c>
       <c r="I2" s="30">
         <v>80</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K2" s="32">
         <v>1</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="65" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G3" s="51" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I3" s="30">
         <v>40</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K3" s="32">
         <v>2</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="65" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F4" s="32"/>
       <c r="H4" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L4" s="31" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="65" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F5" s="32"/>
       <c r="H5" s="32" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="65" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F6" s="32"/>
       <c r="H6" s="32" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="65" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F7" s="32"/>
       <c r="H7" s="32" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="65" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F8" s="32"/>
       <c r="H8" s="32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="65" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F9" s="32"/>
       <c r="H9" s="32" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="65" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="32" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F10" s="32"/>
       <c r="H10" s="32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="65" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F11" s="32"/>
       <c r="H11" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="65" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="32" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F12" s="32"/>
       <c r="H12" s="32" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="65" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B13" s="32"/>
       <c r="C13" s="32" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
       <c r="F13" s="32"/>
       <c r="H13" s="32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="65" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="32" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
       <c r="F14" s="32"/>
       <c r="H14" s="32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H15" s="32" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H16" s="32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H17" s="32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H18" s="32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H19" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H20" s="32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H21" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H22" s="32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H23" s="32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H24" s="32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H25" s="32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H26" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H27" s="32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H28" s="32" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H29" s="32" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H30" s="32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H31" s="32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H32" s="32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H33" s="32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H34" s="32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H35" s="32" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="36" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H36" s="32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="37" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H37" s="32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="38" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H38" s="32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H39" s="32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="40" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H40" s="32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="41" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H41" s="32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="42" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H42" s="32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="43" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H43" s="32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="44" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H44" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="45" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H45" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="46" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H46" s="32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="47" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H47" s="32" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="48" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H48" s="32" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H49" s="32" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="50" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H50" s="32" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="51" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H51" s="32" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="52" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H52" s="32" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="53" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H53" s="32" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="54" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H54" s="32" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="55" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H55" s="32" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="56" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H56" s="32" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="57" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H57" s="32" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="58" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H58" s="32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="59" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H59" s="32" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="60" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H60" s="32" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="61" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H61" s="32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="62" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H62" s="32" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="63" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H63" s="32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="64" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H64" s="32" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="65" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H65" s="32" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="66" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H66" s="32" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="67" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H67" s="32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="68" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H68" s="32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="69" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H69" s="32" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="70" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H70" s="32" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="71" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H71" s="32" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H72" s="32" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H73" s="32" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="74" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H74" s="32" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="75" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H75" s="32" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="76" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H76" s="32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="77" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H77" s="32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="78" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H78" s="32" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="79" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H79" s="32" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="80" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H80" s="32" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="81" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H81" s="32" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="82" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H82" s="32" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="83" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H83" s="32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="84" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H84" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="85" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H85" s="32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="86" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H86" s="32" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="87" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H87" s="32" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="88" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H88" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="89" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H89" s="32" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="90" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H90" s="32" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="91" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H91" s="32" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="92" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H92" s="32" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="93" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H93" s="32" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="94" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H94" s="32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="95" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H95" s="32" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="96" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H96" s="32" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="97" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H97" s="32" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="98" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H98" s="32" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="99" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H99" s="32" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="100" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H100" s="32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="101" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H101" s="32" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="102" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H102" s="32" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="103" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H103" s="32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="104" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H104" s="32" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="105" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H105" s="32" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="106" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H106" s="32" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="107" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H107" s="32" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="108" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H108" s="32" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -38568,91 +38487,91 @@
   <sheetData>
     <row r="1" spans="1:39" s="54" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
+        <v>421</v>
+      </c>
+      <c r="B1" s="62" t="s">
         <v>422</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="C1" s="62" t="s">
         <v>423</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="D1" s="62" t="s">
         <v>424</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="E1" s="62" t="s">
         <v>425</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="F1" s="62" t="s">
         <v>426</v>
-      </c>
-      <c r="F1" s="62" t="s">
-        <v>427</v>
       </c>
       <c r="G1" s="62" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="62" t="s">
+        <v>427</v>
+      </c>
+      <c r="I1" s="62" t="s">
         <v>428</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="J1" s="62" t="s">
         <v>429</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="K1" s="62" t="s">
         <v>430</v>
       </c>
-      <c r="K1" s="62" t="s">
+      <c r="L1" s="62" t="s">
         <v>431</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="M1" s="62" t="s">
+        <v>479</v>
+      </c>
+      <c r="N1" s="62" t="s">
         <v>432</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="O1" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="P1" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q1" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="R1" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="S1" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="T1" s="62" t="s">
+        <v>481</v>
+      </c>
+      <c r="U1" s="62" t="s">
+        <v>438</v>
+      </c>
+      <c r="V1" s="53" t="s">
+        <v>439</v>
+      </c>
+      <c r="W1" s="53" t="s">
+        <v>440</v>
+      </c>
+      <c r="X1" s="53" t="s">
+        <v>441</v>
+      </c>
+      <c r="Y1" s="62" t="s">
         <v>480</v>
-      </c>
-      <c r="N1" s="62" t="s">
-        <v>433</v>
-      </c>
-      <c r="O1" s="62" t="s">
-        <v>434</v>
-      </c>
-      <c r="P1" s="62" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q1" s="62" t="s">
-        <v>436</v>
-      </c>
-      <c r="R1" s="62" t="s">
-        <v>437</v>
-      </c>
-      <c r="S1" s="62" t="s">
-        <v>438</v>
-      </c>
-      <c r="T1" s="62" t="s">
-        <v>482</v>
-      </c>
-      <c r="U1" s="62" t="s">
-        <v>439</v>
-      </c>
-      <c r="V1" s="53" t="s">
-        <v>440</v>
-      </c>
-      <c r="W1" s="53" t="s">
-        <v>441</v>
-      </c>
-      <c r="X1" s="53" t="s">
-        <v>442</v>
-      </c>
-      <c r="Y1" s="62" t="s">
-        <v>481</v>
       </c>
       <c r="Z1" s="53" t="s">
         <v>67</v>
       </c>
       <c r="AA1" s="53" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB1" s="53" t="s">
         <v>443</v>
       </c>
-      <c r="AB1" s="53" t="s">
+      <c r="AC1" s="53" t="s">
         <v>444</v>
-      </c>
-      <c r="AC1" s="53" t="s">
-        <v>445</v>
       </c>
       <c r="AD1" s="53" t="s">
         <v>169</v>
@@ -38673,10 +38592,10 @@
         <v>174</v>
       </c>
       <c r="AJ1" s="53" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="AK1" s="53" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AL1" s="53"/>
       <c r="AM1" s="53"/>
@@ -38705,7 +38624,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="56" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H2" s="56" t="s">
         <v>28</v>
@@ -38728,22 +38647,22 @@
         <v>0</v>
       </c>
       <c r="N2" s="56" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O2" s="56" t="s">
         <v>63</v>
       </c>
       <c r="P2" s="57" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Q2" s="56" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="R2" s="56" t="s">
         <v>42</v>
       </c>
       <c r="S2" s="56" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T2" s="56" cm="1">
         <f t="array" aca="1" ref="T2" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DedicatedVMHosts")&amp;":"&amp;ADDRESS(A2,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A2,3,4,1,"DedicatedVMHosts")))</f>
@@ -38754,13 +38673,13 @@
         <v>0</v>
       </c>
       <c r="V2" s="56" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="W2" s="56" t="s">
         <v>98</v>
       </c>
       <c r="X2" s="56" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="Y2" s="56" t="b">
         <v>1</v>
@@ -38769,7 +38688,7 @@
         <v>108</v>
       </c>
       <c r="AA2" s="56" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AB2" s="56" t="s">
         <v>122</v>
@@ -38799,7 +38718,7 @@
         <v>122</v>
       </c>
       <c r="AK2" s="55" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:39" s="55" customFormat="1" x14ac:dyDescent="0.2">
@@ -38826,7 +38745,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="56" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H3" s="56" t="s">
         <v>27</v>
@@ -38835,7 +38754,7 @@
         <v>42</v>
       </c>
       <c r="J3" s="56" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K3" s="56" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DHCP")&amp;":"&amp;ADDRESS(A3,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A3,4,4,1,"DHCP")))</f>
@@ -38849,10 +38768,10 @@
         <v>0</v>
       </c>
       <c r="N3" s="56" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="O3" s="56" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P3" s="57" t="s">
         <v>64</v>
@@ -38864,7 +38783,7 @@
         <v>69</v>
       </c>
       <c r="S3" s="56" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="T3" s="56" cm="1">
         <f t="array" aca="1" ref="T3" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DedicatedVMHosts")&amp;":"&amp;ADDRESS(A3,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A3,3,4,1,"DedicatedVMHosts")))</f>
@@ -38881,7 +38800,7 @@
         <v>97</v>
       </c>
       <c r="X3" s="56" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="Y3" s="56" t="b">
         <v>0</v>
@@ -38893,7 +38812,7 @@
         <v>121</v>
       </c>
       <c r="AB3" s="56" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="AC3" s="56" t="s">
         <v>123</v>
@@ -38917,10 +38836,10 @@
         <v>16</v>
       </c>
       <c r="AJ3" s="56" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="AK3" s="55" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:39" s="55" customFormat="1" x14ac:dyDescent="0.2">
@@ -38945,7 +38864,7 @@
       </c>
       <c r="F4" s="56"/>
       <c r="G4" s="56" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H4" s="56"/>
       <c r="I4" s="56" t="s">
@@ -38957,7 +38876,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="56" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M4" s="56" cm="1">
         <f t="array" aca="1" ref="M4" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DRGs")&amp;":"&amp;ADDRESS(A4,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A4,3,4,1,"DRGs")))</f>
@@ -38975,7 +38894,7 @@
         <v>76</v>
       </c>
       <c r="S4" s="56" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="T4" s="56" cm="1">
         <f t="array" aca="1" ref="T4" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DedicatedVMHosts")&amp;":"&amp;ADDRESS(A4,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A4,3,4,1,"DedicatedVMHosts")))</f>
@@ -38988,14 +38907,14 @@
       <c r="V4" s="56"/>
       <c r="W4" s="56"/>
       <c r="X4" s="56" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y4" s="56"/>
       <c r="Z4" s="56" t="s">
+        <v>457</v>
+      </c>
+      <c r="AA4" s="56" t="s">
         <v>458</v>
-      </c>
-      <c r="AA4" s="56" t="s">
-        <v>459</v>
       </c>
       <c r="AB4" s="56"/>
       <c r="AC4" s="56" t="s">
@@ -39042,7 +38961,7 @@
       </c>
       <c r="F5" s="56"/>
       <c r="G5" s="56" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H5" s="56"/>
       <c r="I5" s="56" t="s">
@@ -39060,7 +38979,7 @@
       </c>
       <c r="N5" s="56"/>
       <c r="O5" s="56" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="P5" s="57"/>
       <c r="Q5" s="56"/>
@@ -39077,7 +38996,7 @@
       <c r="X5" s="56"/>
       <c r="Y5" s="56"/>
       <c r="Z5" s="56" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AA5" s="56"/>
       <c r="AB5" s="56"/>
@@ -39121,7 +39040,7 @@
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="56" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H6" s="56"/>
       <c r="I6" s="56"/>
@@ -39192,7 +39111,7 @@
       </c>
       <c r="F7" s="56"/>
       <c r="G7" s="56" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H7" s="56"/>
       <c r="I7" s="56"/>
@@ -39261,7 +39180,7 @@
       </c>
       <c r="F8" s="56"/>
       <c r="G8" s="56" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H8" s="56"/>
       <c r="I8" s="56"/>
@@ -39330,7 +39249,7 @@
       </c>
       <c r="F9" s="56"/>
       <c r="G9" s="56" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H9" s="56"/>
       <c r="I9" s="56"/>
@@ -39399,7 +39318,7 @@
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="56" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H10" s="56"/>
       <c r="I10" s="56"/>
@@ -39468,7 +39387,7 @@
       </c>
       <c r="F11" s="56"/>
       <c r="G11" s="56" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H11" s="56"/>
       <c r="I11" s="56"/>
@@ -39537,7 +39456,7 @@
       </c>
       <c r="F12" s="56"/>
       <c r="G12" s="56" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H12" s="56"/>
       <c r="I12" s="56"/>
@@ -39604,7 +39523,7 @@
       </c>
       <c r="F13" s="56"/>
       <c r="G13" s="56" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H13" s="56"/>
       <c r="I13" s="56"/>
@@ -39671,7 +39590,7 @@
       </c>
       <c r="F14" s="56"/>
       <c r="G14" s="56" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H14" s="56"/>
       <c r="I14" s="56"/>
@@ -39805,7 +39724,7 @@
       </c>
       <c r="F16" s="56"/>
       <c r="G16" s="56" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H16" s="56"/>
       <c r="I16" s="56"/>
@@ -39872,7 +39791,7 @@
       </c>
       <c r="F17" s="56"/>
       <c r="G17" s="56" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H17" s="56"/>
       <c r="I17" s="56"/>
@@ -39939,7 +39858,7 @@
       </c>
       <c r="F18" s="56"/>
       <c r="G18" s="56" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H18" s="56"/>
       <c r="I18" s="56"/>
@@ -40006,7 +39925,7 @@
       </c>
       <c r="F19" s="56"/>
       <c r="G19" s="56" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H19" s="56"/>
       <c r="I19" s="56"/>
@@ -40073,7 +39992,7 @@
       </c>
       <c r="F20" s="56"/>
       <c r="G20" s="56" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H20" s="56"/>
       <c r="I20" s="56"/>
@@ -40140,7 +40059,7 @@
       </c>
       <c r="F21" s="56"/>
       <c r="G21" s="56" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H21" s="56"/>
       <c r="I21" s="56"/>
@@ -40207,7 +40126,7 @@
       </c>
       <c r="F22" s="56"/>
       <c r="G22" s="56" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H22" s="56"/>
       <c r="I22" s="56"/>
@@ -40274,7 +40193,7 @@
       </c>
       <c r="F23" s="56"/>
       <c r="G23" s="56" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H23" s="56"/>
       <c r="I23" s="56"/>
@@ -40341,7 +40260,7 @@
       </c>
       <c r="F24" s="56"/>
       <c r="G24" s="56" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H24" s="56"/>
       <c r="I24" s="56"/>
@@ -42114,16 +42033,16 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="53" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="55"/>
       <c r="B2" s="55" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -42589,7 +42508,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="37" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -42622,7 +42541,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -42680,7 +42599,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="169" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -42688,7 +42607,7 @@
       <c r="E1" s="82"/>
       <c r="F1" s="83"/>
       <c r="G1" s="84" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H1" s="85"/>
       <c r="I1" s="85"/>
@@ -42719,7 +42638,7 @@
         <v>215</v>
       </c>
       <c r="I2" s="36" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.2">
@@ -42856,7 +42775,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="31" customFormat="1" ht="187.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -42864,7 +42783,7 @@
       <c r="E1" s="82"/>
       <c r="F1" s="83"/>
       <c r="G1" s="81" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H1" s="82"/>
       <c r="I1" s="82"/>
@@ -42883,7 +42802,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>12</v>
@@ -42907,7 +42826,7 @@
         <v>18</v>
       </c>
       <c r="L2" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -42975,14 +42894,14 @@
   <sheetData>
     <row r="1" spans="1:8" ht="222" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
       <c r="D1" s="80"/>
       <c r="E1" s="80"/>
       <c r="F1" s="86" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
@@ -42995,22 +42914,22 @@
         <v>6</v>
       </c>
       <c r="C2" s="28" t="s">
+        <v>412</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>413</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="E2" s="28" t="s">
         <v>414</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="F2" s="78" t="s">
         <v>415</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="G2" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>417</v>
-      </c>
       <c r="H2" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -43065,7 +42984,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="37" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B1" s="87"/>
     </row>
@@ -43079,19 +42998,19 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B4" s="32"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B5" s="32"/>
     </row>
@@ -43126,7 +43045,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="103.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -43159,7 +43078,7 @@
         <v>26</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.2"/>

</xml_diff>